<commit_message>
Add applyMappingFormat and Complete first set of Climate Dataset! (Missing source_id)
</commit_message>
<xml_diff>
--- a/datasets/Climate-Dataset/1.2_Global_Environmental_Indicators/Air and Climate/NOx_Emissions.xlsx
+++ b/datasets/Climate-Dataset/1.2_Global_Environmental_Indicators/Air and Climate/NOx_Emissions.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Desktop\Data Management\ClimateWaterDataWarehouse\datasets\Climate-Dataset\1.2_Global_Environmental_Indicators\Air and Climate\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2ABB6F8-49CE-4718-88CC-C2C5F13773A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="5208" windowWidth="15480" windowHeight="4212"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -847,9 +866,6 @@
     <t>Panama*</t>
   </si>
   <si>
-    <t>Andorra*</t>
-  </si>
-  <si>
     <t>UN Framework Convention on Climate Change (UNFCCC) Secretariat.</t>
   </si>
   <si>
@@ -978,11 +994,14 @@
   <si>
     <t xml:space="preserve">The latest revision and update of this guideline is 2006 IPCC Guidelines for National Greenhouse Gas Inventories.  In earlier years the guidelines produced for the UNECE Convention on Long Range Transboundary Air Pollution were widely used in Europe, and are still used in some countries.  </t>
   </si>
+  <si>
+    <t>Andorra</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#\ ###\ ##0.00"/>
@@ -1870,13 +1889,13 @@
     <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1907,7 +1926,7 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1935,19 +1954,19 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
@@ -2024,18 +2043,15 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -2052,14 +2068,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -2193,14 +2201,14 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
@@ -2216,11 +2224,7 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -2228,6 +2232,30 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="50" fillId="0" borderId="0" xfId="64" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="64" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -2244,14 +2272,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
@@ -2267,60 +2287,47 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="50" fillId="0" borderId="0" xfId="64" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="64" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="78">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="50"/>
-    <cellStyle name="20% - Accent1 3" xfId="65"/>
+    <cellStyle name="20% - Accent1 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent1 3" xfId="65" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="52"/>
-    <cellStyle name="20% - Accent2 3" xfId="67"/>
+    <cellStyle name="20% - Accent2 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent2 3" xfId="67" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="54"/>
-    <cellStyle name="20% - Accent3 3" xfId="69"/>
+    <cellStyle name="20% - Accent3 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Accent3 3" xfId="69" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="56"/>
-    <cellStyle name="20% - Accent4 3" xfId="71"/>
+    <cellStyle name="20% - Accent4 2" xfId="56" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - Accent4 3" xfId="71" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="58"/>
-    <cellStyle name="20% - Accent5 3" xfId="73"/>
+    <cellStyle name="20% - Accent5 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="20% - Accent5 3" xfId="73" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 2" xfId="60"/>
-    <cellStyle name="20% - Accent6 3" xfId="75"/>
+    <cellStyle name="20% - Accent6 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="20% - Accent6 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="51"/>
-    <cellStyle name="40% - Accent1 3" xfId="66"/>
+    <cellStyle name="40% - Accent1 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="40% - Accent1 3" xfId="66" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
     <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="53"/>
-    <cellStyle name="40% - Accent2 3" xfId="68"/>
+    <cellStyle name="40% - Accent2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="40% - Accent2 3" xfId="68" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="55"/>
-    <cellStyle name="40% - Accent3 3" xfId="70"/>
+    <cellStyle name="40% - Accent3 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="40% - Accent3 3" xfId="70" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
     <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="57"/>
-    <cellStyle name="40% - Accent4 3" xfId="72"/>
+    <cellStyle name="40% - Accent4 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="40% - Accent4 3" xfId="72" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
     <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="59"/>
-    <cellStyle name="40% - Accent5 3" xfId="74"/>
+    <cellStyle name="40% - Accent5 2" xfId="59" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="40% - Accent5 3" xfId="74" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="61"/>
-    <cellStyle name="40% - Accent6 3" xfId="76"/>
+    <cellStyle name="40% - Accent6 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="40% - Accent6 3" xfId="76" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
     <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
@@ -2347,18 +2354,18 @@
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="43"/>
-    <cellStyle name="Normal 2 2" xfId="63"/>
-    <cellStyle name="Normal 2 3" xfId="46"/>
-    <cellStyle name="Normal 3" xfId="47"/>
-    <cellStyle name="Normal 4" xfId="48"/>
-    <cellStyle name="Normal 5" xfId="45"/>
-    <cellStyle name="Normal 6" xfId="44"/>
-    <cellStyle name="Normal_Sheet1" xfId="1"/>
-    <cellStyle name="Note 2" xfId="42"/>
-    <cellStyle name="Note 2 2" xfId="62"/>
-    <cellStyle name="Note 2 3" xfId="77"/>
-    <cellStyle name="Note 3" xfId="49"/>
+    <cellStyle name="Normal 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Normal 2 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Normal 2 3" xfId="46" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Normal 3" xfId="47" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Normal 4" xfId="48" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Normal 5" xfId="45" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Normal 6" xfId="44" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Note 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Note 2 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Note 2 3" xfId="77" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Note 3" xfId="49" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
     <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
@@ -2370,14 +2377,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2415,7 +2425,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2487,7 +2497,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2660,31 +2670,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="18" topLeftCell="A19" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="18" topLeftCell="A22" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.5546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="39.44140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="8"/>
-    <col min="4" max="4" width="13.33203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="2.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" style="16" customWidth="1"/>
-    <col min="7" max="7" width="2.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="15" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="8"/>
+    <col min="4" max="4" width="13.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="15" customWidth="1"/>
     <col min="9" max="9" width="3" style="8" customWidth="1"/>
-    <col min="10" max="10" width="0.88671875" style="8" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="8"/>
+    <col min="10" max="10" width="0.85546875" style="8" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2696,7 +2706,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>138</v>
@@ -2710,7 +2720,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="9"/>
       <c r="C4" s="5"/>
@@ -2722,7 +2732,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="10" t="s">
         <v>153</v>
@@ -2733,12 +2743,12 @@
       <c r="F5" s="7"/>
       <c r="G5" s="3"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="86" t="s">
-        <v>196</v>
+      <c r="I5" s="83" t="s">
+        <v>195</v>
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="10"/>
       <c r="C6" s="5"/>
@@ -2750,7 +2760,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="4" t="s">
         <v>140</v>
@@ -2758,15 +2768,15 @@
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="100"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="10"/>
       <c r="C8" s="5"/>
@@ -2778,95 +2788,95 @@
       <c r="I8" s="11"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="21.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="66"/>
-      <c r="F9" s="67" t="s">
+      <c r="E9" s="63"/>
+      <c r="F9" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="68"/>
-      <c r="H9" s="65" t="s">
+      <c r="G9" s="65"/>
+      <c r="H9" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="I9" s="69"/>
+      <c r="I9" s="66"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72" t="s">
+      <c r="B10" s="67"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="74" t="s">
+      <c r="E10" s="70"/>
+      <c r="F10" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="75"/>
-      <c r="H10" s="72" t="s">
+      <c r="G10" s="72"/>
+      <c r="H10" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="76"/>
+      <c r="I10" s="73"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
-      <c r="B11" s="85" t="str">
+      <c r="B11" s="82" t="str">
         <f>F7</f>
         <v>Afghanistan</v>
       </c>
-      <c r="C11" s="77">
+      <c r="C11" s="74">
         <f>VLOOKUP(F7,B19:I183,2,TRUE)</f>
         <v>2005</v>
       </c>
-      <c r="D11" s="78">
+      <c r="D11" s="75">
         <f>VLOOKUP(F7,B19:I183,3,TRUE)</f>
         <v>62.58</v>
       </c>
-      <c r="E11" s="90" t="str">
+      <c r="E11" s="87" t="str">
         <f>IF((VLOOKUP(F7,B19:I183,4,TRUE))="","",(VLOOKUP(F7,B19:I183,4,TRUE)))</f>
         <v/>
       </c>
-      <c r="F11" s="79" t="str">
+      <c r="F11" s="76" t="str">
         <f>VLOOKUP(F7,B19:I183,5,TRUE)</f>
         <v>…</v>
       </c>
-      <c r="G11" s="90" t="str">
+      <c r="G11" s="87" t="str">
         <f>IF((VLOOKUP(F7,B19:I183,6,TRUE))="","",(VLOOKUP(F7,B19:I183,6,TRUE)))</f>
         <v/>
       </c>
-      <c r="H11" s="78">
+      <c r="H11" s="75">
         <f>VLOOKUP(F7,B19:I183,7,TRUE)</f>
         <v>2.5647595642416943</v>
       </c>
-      <c r="I11" s="89" t="str">
+      <c r="I11" s="86" t="str">
         <f>IF((VLOOKUP(F7,B19:I183,8,TRUE))="","",(VLOOKUP(F7,B19:I183,8,TRUE)))</f>
         <v/>
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="80"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="83"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -2875,12 +2885,12 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="84" t="s">
+      <c r="I13" s="81" t="s">
         <v>141</v>
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
@@ -2892,19 +2902,19 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="1.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="1.1499999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G15" s="17"/>
-      <c r="H15" s="100"/>
-      <c r="I15" s="100"/>
-    </row>
-    <row r="16" spans="1:10" ht="1.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="101"/>
+      <c r="I15" s="101"/>
+    </row>
+    <row r="16" spans="1:10" ht="1.1499999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D16" s="18"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22"/>
       <c r="B17" s="2" t="s">
         <v>139</v>
@@ -2926,7 +2936,7 @@
       <c r="I17" s="22"/>
       <c r="J17" s="22"/>
     </row>
-    <row r="18" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28"/>
       <c r="B18" s="29"/>
       <c r="C18" s="30"/>
@@ -2944,7 +2954,7 @@
       <c r="I18" s="35"/>
       <c r="J18" s="28"/>
     </row>
-    <row r="19" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="37" t="s">
         <v>155</v>
@@ -2966,7 +2976,7 @@
       <c r="I19" s="41"/>
       <c r="J19" s="40"/>
     </row>
-    <row r="20" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="36"/>
       <c r="B20" s="37" t="s">
         <v>5</v>
@@ -2988,7 +2998,7 @@
       <c r="I20" s="41"/>
       <c r="J20" s="40"/>
     </row>
-    <row r="21" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36"/>
       <c r="B21" s="37" t="s">
         <v>6</v>
@@ -3010,10 +3020,10 @@
       <c r="I21" s="41"/>
       <c r="J21" s="40"/>
     </row>
-    <row r="22" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36"/>
-      <c r="B22" s="37" t="s">
-        <v>192</v>
+      <c r="B22" s="106" t="s">
+        <v>203</v>
       </c>
       <c r="C22" s="37">
         <v>1997</v>
@@ -3036,7 +3046,7 @@
       </c>
       <c r="J22" s="40"/>
     </row>
-    <row r="23" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36"/>
       <c r="B23" s="37" t="s">
         <v>156</v>
@@ -3058,7 +3068,7 @@
       <c r="I23" s="41"/>
       <c r="J23" s="40"/>
     </row>
-    <row r="24" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="42" t="s">
         <v>157</v>
       </c>
@@ -3068,18 +3078,18 @@
       <c r="D24" s="43">
         <v>2.27</v>
       </c>
-      <c r="E24" s="87"/>
+      <c r="E24" s="84"/>
       <c r="F24" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G24" s="87"/>
+      <c r="G24" s="84"/>
       <c r="H24" s="43">
         <v>29.234494127343915</v>
       </c>
-      <c r="I24" s="87"/>
-      <c r="J24" s="46"/>
-    </row>
-    <row r="25" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="84"/>
+      <c r="J24" s="45"/>
+    </row>
+    <row r="25" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="42" t="s">
         <v>7</v>
       </c>
@@ -3089,18 +3099,18 @@
       <c r="D25" s="43">
         <v>675.79175783000403</v>
       </c>
-      <c r="E25" s="87"/>
+      <c r="E25" s="84"/>
       <c r="F25" s="44">
         <v>31.128567597557339</v>
       </c>
-      <c r="G25" s="87"/>
+      <c r="G25" s="84"/>
       <c r="H25" s="43">
         <v>18.236325033725443</v>
       </c>
-      <c r="I25" s="87"/>
-      <c r="J25" s="46"/>
-    </row>
-    <row r="26" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="84"/>
+      <c r="J25" s="45"/>
+    </row>
+    <row r="26" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="42" t="s">
         <v>8</v>
       </c>
@@ -3110,18 +3120,18 @@
       <c r="D26" s="43">
         <v>17.213000000000001</v>
       </c>
-      <c r="E26" s="87"/>
+      <c r="E26" s="84"/>
       <c r="F26" s="44">
         <v>-77.525786656221442</v>
       </c>
-      <c r="G26" s="87"/>
+      <c r="G26" s="84"/>
       <c r="H26" s="43">
         <v>5.8083425791700076</v>
       </c>
-      <c r="I26" s="87"/>
-      <c r="J26" s="46"/>
-    </row>
-    <row r="27" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="84"/>
+      <c r="J26" s="45"/>
+    </row>
+    <row r="27" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="42" t="s">
         <v>9</v>
       </c>
@@ -3131,18 +3141,18 @@
       <c r="D27" s="43">
         <v>2536.45357023724</v>
       </c>
-      <c r="E27" s="87"/>
+      <c r="E27" s="84"/>
       <c r="F27" s="44">
         <v>44.596297898558035</v>
       </c>
-      <c r="G27" s="87"/>
+      <c r="G27" s="84"/>
       <c r="H27" s="43">
         <v>110.70717363044513</v>
       </c>
-      <c r="I27" s="87"/>
-      <c r="J27" s="46"/>
-    </row>
-    <row r="28" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="84"/>
+      <c r="J27" s="45"/>
+    </row>
+    <row r="28" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="42" t="s">
         <v>10</v>
       </c>
@@ -3152,18 +3162,18 @@
       <c r="D28" s="43">
         <v>178.262141211357</v>
       </c>
-      <c r="E28" s="87"/>
+      <c r="E28" s="84"/>
       <c r="F28" s="44">
         <v>-8.4616072379727871</v>
       </c>
-      <c r="G28" s="87"/>
+      <c r="G28" s="84"/>
       <c r="H28" s="43">
         <v>21.082446467698627</v>
       </c>
-      <c r="I28" s="87"/>
-      <c r="J28" s="46"/>
-    </row>
-    <row r="29" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="84"/>
+      <c r="J28" s="45"/>
+    </row>
+    <row r="29" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="36"/>
       <c r="B29" s="37" t="s">
         <v>158</v>
@@ -3185,7 +3195,7 @@
       <c r="I29" s="41"/>
       <c r="J29" s="40"/>
     </row>
-    <row r="30" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36"/>
       <c r="B30" s="37" t="s">
         <v>11</v>
@@ -3207,7 +3217,7 @@
       <c r="I30" s="41"/>
       <c r="J30" s="40"/>
     </row>
-    <row r="31" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36"/>
       <c r="B31" s="37" t="s">
         <v>159</v>
@@ -3229,7 +3239,7 @@
       <c r="I31" s="41"/>
       <c r="J31" s="40"/>
     </row>
-    <row r="32" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36"/>
       <c r="B32" s="37" t="s">
         <v>12</v>
@@ -3251,7 +3261,7 @@
       <c r="I32" s="41"/>
       <c r="J32" s="40"/>
     </row>
-    <row r="33" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="36"/>
       <c r="B33" s="37" t="s">
         <v>13</v>
@@ -3273,7 +3283,7 @@
       <c r="I33" s="41"/>
       <c r="J33" s="40"/>
     </row>
-    <row r="34" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="42" t="s">
         <v>14</v>
       </c>
@@ -3283,18 +3293,18 @@
       <c r="D34" s="43">
         <v>193.30865060683101</v>
       </c>
-      <c r="E34" s="87"/>
+      <c r="E34" s="84"/>
       <c r="F34" s="44">
         <v>-47.941228629985957</v>
       </c>
-      <c r="G34" s="87"/>
+      <c r="G34" s="84"/>
       <c r="H34" s="43">
         <v>17.447383384789919</v>
       </c>
-      <c r="I34" s="87"/>
-      <c r="J34" s="46"/>
-    </row>
-    <row r="35" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="84"/>
+      <c r="J34" s="45"/>
+    </row>
+    <row r="35" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="42" t="s">
         <v>15</v>
       </c>
@@ -3304,18 +3314,18 @@
       <c r="D35" s="43">
         <v>5.5970000000000004</v>
       </c>
-      <c r="E35" s="87"/>
+      <c r="E35" s="84"/>
       <c r="F35" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G35" s="87"/>
+      <c r="G35" s="84"/>
       <c r="H35" s="43">
         <v>27.75215938277849</v>
       </c>
-      <c r="I35" s="87"/>
-      <c r="J35" s="46"/>
-    </row>
-    <row r="36" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="84"/>
+      <c r="J35" s="45"/>
+    </row>
+    <row r="36" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="42" t="s">
         <v>16</v>
       </c>
@@ -3325,18 +3335,18 @@
       <c r="D36" s="43">
         <v>60.526000000000003</v>
       </c>
-      <c r="E36" s="87"/>
+      <c r="E36" s="84"/>
       <c r="F36" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G36" s="87"/>
+      <c r="G36" s="84"/>
       <c r="H36" s="43">
         <v>8.709571491845443</v>
       </c>
-      <c r="I36" s="87"/>
-      <c r="J36" s="46"/>
-    </row>
-    <row r="37" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="84"/>
+      <c r="J36" s="45"/>
+    </row>
+    <row r="37" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="42" t="s">
         <v>17</v>
       </c>
@@ -3346,18 +3356,18 @@
       <c r="D37" s="43">
         <v>1.77</v>
       </c>
-      <c r="E37" s="87"/>
+      <c r="E37" s="84"/>
       <c r="F37" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G37" s="87"/>
+      <c r="G37" s="84"/>
       <c r="H37" s="43">
         <v>3.1372576822932823</v>
       </c>
-      <c r="I37" s="87"/>
-      <c r="J37" s="46"/>
-    </row>
-    <row r="38" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="84"/>
+      <c r="J37" s="45"/>
+    </row>
+    <row r="38" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="42" t="s">
         <v>160</v>
       </c>
@@ -3367,18 +3377,18 @@
       <c r="D38" s="43">
         <v>64.919740000000004</v>
       </c>
-      <c r="E38" s="87"/>
+      <c r="E38" s="84"/>
       <c r="F38" s="44">
         <v>31.071552594387246</v>
       </c>
-      <c r="G38" s="87"/>
+      <c r="G38" s="84"/>
       <c r="H38" s="43">
         <v>7.2392531451625501</v>
       </c>
-      <c r="I38" s="87"/>
-      <c r="J38" s="46"/>
-    </row>
-    <row r="39" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="84"/>
+      <c r="J38" s="45"/>
+    </row>
+    <row r="39" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="36"/>
       <c r="B39" s="37" t="s">
         <v>161</v>
@@ -3400,7 +3410,7 @@
       <c r="I39" s="41"/>
       <c r="J39" s="40"/>
     </row>
-    <row r="40" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="36"/>
       <c r="B40" s="37" t="s">
         <v>18</v>
@@ -3422,7 +3432,7 @@
       <c r="I40" s="41"/>
       <c r="J40" s="40"/>
     </row>
-    <row r="41" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="36"/>
       <c r="B41" s="37" t="s">
         <v>19</v>
@@ -3444,7 +3454,7 @@
       <c r="I41" s="41"/>
       <c r="J41" s="40"/>
     </row>
-    <row r="42" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="36"/>
       <c r="B42" s="37" t="s">
         <v>20</v>
@@ -3466,7 +3476,7 @@
       <c r="I42" s="41"/>
       <c r="J42" s="40"/>
     </row>
-    <row r="43" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="36"/>
       <c r="B43" s="37" t="s">
         <v>21</v>
@@ -3488,7 +3498,7 @@
       <c r="I43" s="41"/>
       <c r="J43" s="40"/>
     </row>
-    <row r="44" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="42" t="s">
         <v>162</v>
       </c>
@@ -3498,18 +3508,18 @@
       <c r="D44" s="43">
         <v>2.0270000000000001</v>
       </c>
-      <c r="E44" s="87"/>
+      <c r="E44" s="84"/>
       <c r="F44" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G44" s="87"/>
+      <c r="G44" s="84"/>
       <c r="H44" s="43">
         <v>4.6200799111996478</v>
       </c>
-      <c r="I44" s="87"/>
-      <c r="J44" s="46"/>
-    </row>
-    <row r="45" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I44" s="84"/>
+      <c r="J44" s="45"/>
+    </row>
+    <row r="45" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="42" t="s">
         <v>22</v>
       </c>
@@ -3519,18 +3529,18 @@
       <c r="D45" s="43">
         <v>38.020000000000003</v>
       </c>
-      <c r="E45" s="87"/>
+      <c r="E45" s="84"/>
       <c r="F45" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G45" s="87"/>
+      <c r="G45" s="84"/>
       <c r="H45" s="43">
         <v>3.6715664986649772</v>
       </c>
-      <c r="I45" s="87"/>
-      <c r="J45" s="46"/>
-    </row>
-    <row r="46" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="84"/>
+      <c r="J45" s="45"/>
+    </row>
+    <row r="46" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="42" t="s">
         <v>23</v>
       </c>
@@ -3540,18 +3550,18 @@
       <c r="D46" s="43">
         <v>252.22</v>
       </c>
-      <c r="E46" s="87"/>
+      <c r="E46" s="84"/>
       <c r="F46" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G46" s="87"/>
+      <c r="G46" s="84"/>
       <c r="H46" s="43">
         <v>18.618387499415913</v>
       </c>
-      <c r="I46" s="87"/>
-      <c r="J46" s="46"/>
-    </row>
-    <row r="47" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="84"/>
+      <c r="J46" s="45"/>
+    </row>
+    <row r="47" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="42" t="s">
         <v>24</v>
       </c>
@@ -3561,18 +3571,18 @@
       <c r="D47" s="43">
         <v>51.246000000000002</v>
       </c>
-      <c r="E47" s="87"/>
+      <c r="E47" s="84"/>
       <c r="F47" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G47" s="87"/>
+      <c r="G47" s="84"/>
       <c r="H47" s="43">
         <v>15.750078833376671</v>
       </c>
-      <c r="I47" s="87"/>
-      <c r="J47" s="46"/>
-    </row>
-    <row r="48" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I47" s="84"/>
+      <c r="J47" s="45"/>
+    </row>
+    <row r="48" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="42" t="s">
         <v>25</v>
       </c>
@@ -3582,18 +3592,18 @@
       <c r="D48" s="43">
         <v>78.349999999999994</v>
       </c>
-      <c r="E48" s="87"/>
+      <c r="E48" s="84"/>
       <c r="F48" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G48" s="87"/>
+      <c r="G48" s="84"/>
       <c r="H48" s="43">
         <v>11.949740018802347</v>
       </c>
-      <c r="I48" s="87"/>
-      <c r="J48" s="46"/>
-    </row>
-    <row r="49" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="84"/>
+      <c r="J48" s="45"/>
+    </row>
+    <row r="49" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="36"/>
       <c r="B49" s="37" t="s">
         <v>26</v>
@@ -3615,7 +3625,7 @@
       <c r="I49" s="41"/>
       <c r="J49" s="40"/>
     </row>
-    <row r="50" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="36"/>
       <c r="B50" s="37" t="s">
         <v>27</v>
@@ -3637,7 +3647,7 @@
       <c r="I50" s="41"/>
       <c r="J50" s="40"/>
     </row>
-    <row r="51" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="36"/>
       <c r="B51" s="37" t="s">
         <v>28</v>
@@ -3659,7 +3669,7 @@
       <c r="I51" s="41"/>
       <c r="J51" s="40"/>
     </row>
-    <row r="52" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="36"/>
       <c r="B52" s="37" t="s">
         <v>29</v>
@@ -3681,7 +3691,7 @@
       <c r="I52" s="41"/>
       <c r="J52" s="40"/>
     </row>
-    <row r="53" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="36"/>
       <c r="B53" s="37" t="s">
         <v>30</v>
@@ -3703,7 +3713,7 @@
       <c r="I53" s="41"/>
       <c r="J53" s="40"/>
     </row>
-    <row r="54" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="42" t="s">
         <v>184</v>
       </c>
@@ -3713,18 +3723,18 @@
       <c r="D54" s="43">
         <v>290.49</v>
       </c>
-      <c r="E54" s="87"/>
+      <c r="E54" s="84"/>
       <c r="F54" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G54" s="87"/>
+      <c r="G54" s="84"/>
       <c r="H54" s="43">
         <v>17.586324887328622</v>
       </c>
-      <c r="I54" s="87"/>
-      <c r="J54" s="46"/>
-    </row>
-    <row r="55" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I54" s="84"/>
+      <c r="J54" s="45"/>
+    </row>
+    <row r="55" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="42" t="s">
         <v>31</v>
       </c>
@@ -3734,18 +3744,18 @@
       <c r="D55" s="43">
         <v>55.19</v>
       </c>
-      <c r="E55" s="87"/>
+      <c r="E55" s="84"/>
       <c r="F55" s="44">
         <v>-40.851522596774963</v>
       </c>
-      <c r="G55" s="87"/>
+      <c r="G55" s="84"/>
       <c r="H55" s="43">
         <v>12.873759480664283</v>
       </c>
-      <c r="I55" s="87"/>
-      <c r="J55" s="46"/>
-    </row>
-    <row r="56" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I55" s="84"/>
+      <c r="J55" s="45"/>
+    </row>
+    <row r="56" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="42" t="s">
         <v>32</v>
       </c>
@@ -3755,18 +3765,18 @@
       <c r="D56" s="43">
         <v>101.54</v>
       </c>
-      <c r="E56" s="87"/>
+      <c r="E56" s="84"/>
       <c r="F56" s="44">
         <v>-28.351679367767424</v>
       </c>
-      <c r="G56" s="87"/>
+      <c r="G56" s="84"/>
       <c r="H56" s="43">
         <v>9.2685122878529373</v>
       </c>
-      <c r="I56" s="87"/>
-      <c r="J56" s="46"/>
-    </row>
-    <row r="57" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I56" s="84"/>
+      <c r="J56" s="45"/>
+    </row>
+    <row r="57" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="42" t="s">
         <v>163</v>
       </c>
@@ -3776,18 +3786,18 @@
       <c r="D57" s="43">
         <v>2124</v>
       </c>
-      <c r="E57" s="87"/>
-      <c r="F57" s="95">
+      <c r="E57" s="84"/>
+      <c r="F57" s="90">
         <v>13321.342547001268</v>
       </c>
-      <c r="G57" s="87"/>
+      <c r="G57" s="84"/>
       <c r="H57" s="43">
         <v>1880.8061255482362</v>
       </c>
-      <c r="I57" s="87"/>
-      <c r="J57" s="46"/>
-    </row>
-    <row r="58" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I57" s="84"/>
+      <c r="J57" s="45"/>
+    </row>
+    <row r="58" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="42" t="s">
         <v>33</v>
       </c>
@@ -3797,18 +3807,18 @@
       <c r="D58" s="43">
         <v>210.77</v>
       </c>
-      <c r="E58" s="87"/>
+      <c r="E58" s="84"/>
       <c r="F58" s="44">
         <v>-71.607212407120244</v>
       </c>
-      <c r="G58" s="87"/>
+      <c r="G58" s="84"/>
       <c r="H58" s="43">
         <v>19.987366717302848</v>
       </c>
-      <c r="I58" s="87"/>
-      <c r="J58" s="46"/>
-    </row>
-    <row r="59" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I58" s="84"/>
+      <c r="J58" s="45"/>
+    </row>
+    <row r="59" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="36"/>
       <c r="B59" s="37" t="s">
         <v>164</v>
@@ -3830,7 +3840,7 @@
       <c r="I59" s="41"/>
       <c r="J59" s="40"/>
     </row>
-    <row r="60" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="36"/>
       <c r="B60" s="37" t="s">
         <v>165</v>
@@ -3852,7 +3862,7 @@
       <c r="I60" s="41"/>
       <c r="J60" s="40"/>
     </row>
-    <row r="61" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="36"/>
       <c r="B61" s="37" t="s">
         <v>34</v>
@@ -3874,7 +3884,7 @@
       <c r="I61" s="41"/>
       <c r="J61" s="40"/>
     </row>
-    <row r="62" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="36"/>
       <c r="B62" s="37" t="s">
         <v>35</v>
@@ -3896,7 +3906,7 @@
       <c r="I62" s="41"/>
       <c r="J62" s="40"/>
     </row>
-    <row r="63" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="36"/>
       <c r="B63" s="37" t="s">
         <v>36</v>
@@ -3918,7 +3928,7 @@
       <c r="I63" s="41"/>
       <c r="J63" s="40"/>
     </row>
-    <row r="64" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="42" t="s">
         <v>37</v>
       </c>
@@ -3928,18 +3938,18 @@
       <c r="D64" s="43">
         <v>93.12</v>
       </c>
-      <c r="E64" s="87"/>
+      <c r="E64" s="84"/>
       <c r="F64" s="44">
         <v>68.329718004338403</v>
       </c>
-      <c r="G64" s="87"/>
+      <c r="G64" s="84"/>
       <c r="H64" s="43">
         <v>10.875172245700881</v>
       </c>
-      <c r="I64" s="87"/>
-      <c r="J64" s="46"/>
-    </row>
-    <row r="65" spans="1:10" s="47" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I64" s="84"/>
+      <c r="J64" s="45"/>
+    </row>
+    <row r="65" spans="1:10" s="46" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8"/>
       <c r="B65" s="42" t="s">
         <v>38</v>
@@ -3950,18 +3960,18 @@
       <c r="D65" s="43">
         <v>231.77</v>
       </c>
-      <c r="E65" s="87"/>
+      <c r="E65" s="84"/>
       <c r="F65" s="44">
         <v>47.708877700592708</v>
       </c>
-      <c r="G65" s="87"/>
+      <c r="G65" s="84"/>
       <c r="H65" s="43">
         <v>16.593532553092935</v>
       </c>
-      <c r="I65" s="87"/>
-      <c r="J65" s="46"/>
-    </row>
-    <row r="66" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I65" s="84"/>
+      <c r="J65" s="45"/>
+    </row>
+    <row r="66" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="42" t="s">
         <v>39</v>
       </c>
@@ -3971,18 +3981,18 @@
       <c r="D66" s="43">
         <v>40.42</v>
       </c>
-      <c r="E66" s="87"/>
+      <c r="E66" s="84"/>
       <c r="F66" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="87"/>
+      <c r="G66" s="84"/>
       <c r="H66" s="43">
         <v>6.7964687955991439</v>
       </c>
-      <c r="I66" s="87"/>
-      <c r="J66" s="46"/>
-    </row>
-    <row r="67" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I66" s="84"/>
+      <c r="J66" s="45"/>
+    </row>
+    <row r="67" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="42" t="s">
         <v>40</v>
       </c>
@@ -3992,18 +4002,18 @@
       <c r="D67" s="43">
         <v>6</v>
       </c>
-      <c r="E67" s="87"/>
+      <c r="E67" s="84"/>
       <c r="F67" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G67" s="87"/>
+      <c r="G67" s="84"/>
       <c r="H67" s="43">
         <v>1.697237689086422</v>
       </c>
-      <c r="I67" s="87"/>
-      <c r="J67" s="46"/>
-    </row>
-    <row r="68" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I67" s="84"/>
+      <c r="J67" s="45"/>
+    </row>
+    <row r="68" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="42" t="s">
         <v>41</v>
       </c>
@@ -4013,18 +4023,18 @@
       <c r="D68" s="43">
         <v>3182</v>
       </c>
-      <c r="E68" s="87"/>
-      <c r="F68" s="95">
+      <c r="E68" s="84"/>
+      <c r="F68" s="90">
         <v>4021.8095470872513</v>
       </c>
-      <c r="G68" s="87"/>
+      <c r="G68" s="84"/>
       <c r="H68" s="43">
         <v>2403.2506570798464</v>
       </c>
-      <c r="I68" s="87"/>
-      <c r="J68" s="46"/>
-    </row>
-    <row r="69" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I68" s="84"/>
+      <c r="J68" s="45"/>
+    </row>
+    <row r="69" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="36"/>
       <c r="B69" s="37" t="s">
         <v>42</v>
@@ -4046,7 +4056,7 @@
       <c r="I69" s="41"/>
       <c r="J69" s="40"/>
     </row>
-    <row r="70" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="36"/>
       <c r="B70" s="37" t="s">
         <v>43</v>
@@ -4068,7 +4078,7 @@
       <c r="I70" s="41"/>
       <c r="J70" s="40"/>
     </row>
-    <row r="71" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="36"/>
       <c r="B71" s="37" t="s">
         <v>44</v>
@@ -4090,7 +4100,7 @@
       <c r="I71" s="41"/>
       <c r="J71" s="40"/>
     </row>
-    <row r="72" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="36"/>
       <c r="B72" s="37" t="s">
         <v>45</v>
@@ -4112,7 +4122,7 @@
       <c r="I72" s="41"/>
       <c r="J72" s="40"/>
     </row>
-    <row r="73" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="36"/>
       <c r="B73" s="37" t="s">
         <v>46</v>
@@ -4134,7 +4144,7 @@
       <c r="I73" s="41"/>
       <c r="J73" s="40"/>
     </row>
-    <row r="74" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="42" t="s">
         <v>47</v>
       </c>
@@ -4144,18 +4154,18 @@
       <c r="D74" s="43">
         <v>6.8339999999999996</v>
       </c>
-      <c r="E74" s="87"/>
+      <c r="E74" s="84"/>
       <c r="F74" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G74" s="87"/>
+      <c r="G74" s="84"/>
       <c r="H74" s="43">
         <v>5.5612383154183984</v>
       </c>
-      <c r="I74" s="87"/>
-      <c r="J74" s="46"/>
-    </row>
-    <row r="75" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I74" s="84"/>
+      <c r="J74" s="45"/>
+    </row>
+    <row r="75" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="42" t="s">
         <v>142</v>
       </c>
@@ -4165,18 +4175,18 @@
       <c r="D75" s="43">
         <v>27.67</v>
       </c>
-      <c r="E75" s="87"/>
+      <c r="E75" s="84"/>
       <c r="F75" s="44">
         <v>-78.633567615067534</v>
       </c>
-      <c r="G75" s="87"/>
+      <c r="G75" s="84"/>
       <c r="H75" s="43">
         <v>6.2471975663248287</v>
       </c>
-      <c r="I75" s="87"/>
-      <c r="J75" s="46"/>
-    </row>
-    <row r="76" spans="1:10" s="47" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I75" s="84"/>
+      <c r="J75" s="45"/>
+    </row>
+    <row r="76" spans="1:10" s="46" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
       <c r="B76" s="42" t="s">
         <v>48</v>
@@ -4187,18 +4197,18 @@
       <c r="D76" s="43">
         <v>1269.26</v>
       </c>
-      <c r="E76" s="87"/>
+      <c r="E76" s="84"/>
       <c r="F76" s="44">
         <v>-55.881778201891819</v>
       </c>
-      <c r="G76" s="87"/>
+      <c r="G76" s="84"/>
       <c r="H76" s="43">
         <v>15.771524603409391</v>
       </c>
-      <c r="I76" s="87"/>
-      <c r="J76" s="46"/>
-    </row>
-    <row r="77" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I76" s="84"/>
+      <c r="J76" s="45"/>
+    </row>
+    <row r="77" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="42" t="s">
         <v>166</v>
       </c>
@@ -4208,18 +4218,18 @@
       <c r="D77" s="43">
         <v>205.64</v>
       </c>
-      <c r="E77" s="87"/>
+      <c r="E77" s="84"/>
       <c r="F77" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G77" s="87"/>
+      <c r="G77" s="84"/>
       <c r="H77" s="43">
         <v>10.92377506202658</v>
       </c>
-      <c r="I77" s="87"/>
-      <c r="J77" s="46"/>
-    </row>
-    <row r="78" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I77" s="84"/>
+      <c r="J77" s="45"/>
+    </row>
+    <row r="78" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="42" t="s">
         <v>49</v>
       </c>
@@ -4229,18 +4239,18 @@
       <c r="D78" s="43">
         <v>258.91197769061102</v>
       </c>
-      <c r="E78" s="87"/>
+      <c r="E78" s="84"/>
       <c r="F78" s="44">
         <v>-20.630005890151747</v>
       </c>
-      <c r="G78" s="87"/>
+      <c r="G78" s="84"/>
       <c r="H78" s="43">
         <v>23.305117445572243</v>
       </c>
-      <c r="I78" s="87"/>
-      <c r="J78" s="46"/>
-    </row>
-    <row r="79" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I78" s="84"/>
+      <c r="J78" s="45"/>
+    </row>
+    <row r="79" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="36"/>
       <c r="B79" s="37" t="s">
         <v>50</v>
@@ -4262,7 +4272,7 @@
       <c r="I79" s="41"/>
       <c r="J79" s="40"/>
     </row>
-    <row r="80" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="36"/>
       <c r="B80" s="37" t="s">
         <v>51</v>
@@ -4284,7 +4294,7 @@
       <c r="I80" s="41"/>
       <c r="J80" s="40"/>
     </row>
-    <row r="81" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="36"/>
       <c r="B81" s="37" t="s">
         <v>52</v>
@@ -4306,7 +4316,7 @@
       <c r="I81" s="41"/>
       <c r="J81" s="40"/>
     </row>
-    <row r="82" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="36"/>
       <c r="B82" s="37" t="s">
         <v>53</v>
@@ -4328,7 +4338,7 @@
       <c r="I82" s="41"/>
       <c r="J82" s="40"/>
     </row>
-    <row r="83" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="36"/>
       <c r="B83" s="37" t="s">
         <v>54</v>
@@ -4350,7 +4360,7 @@
       <c r="I83" s="41"/>
       <c r="J83" s="40"/>
     </row>
-    <row r="84" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="42" t="s">
         <v>55</v>
       </c>
@@ -4360,18 +4370,18 @@
       <c r="D84" s="43">
         <v>47.77</v>
       </c>
-      <c r="E84" s="87"/>
+      <c r="E84" s="84"/>
       <c r="F84" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G84" s="87"/>
+      <c r="G84" s="84"/>
       <c r="H84" s="43">
         <v>7.6516719311621832</v>
       </c>
-      <c r="I84" s="87"/>
-      <c r="J84" s="46"/>
-    </row>
-    <row r="85" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I84" s="84"/>
+      <c r="J84" s="45"/>
+    </row>
+    <row r="85" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="42" t="s">
         <v>56</v>
       </c>
@@ -4381,20 +4391,20 @@
       <c r="D85" s="43">
         <v>109.414310217398</v>
       </c>
-      <c r="E85" s="87"/>
+      <c r="E85" s="84"/>
       <c r="F85" s="44">
         <v>-53.01626884075452</v>
       </c>
-      <c r="G85" s="87">
+      <c r="G85" s="84">
         <v>2</v>
       </c>
       <c r="H85" s="43">
         <v>10.987210332310404</v>
       </c>
-      <c r="I85" s="87"/>
-      <c r="J85" s="46"/>
-    </row>
-    <row r="86" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I85" s="84"/>
+      <c r="J85" s="45"/>
+    </row>
+    <row r="86" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="42" t="s">
         <v>57</v>
       </c>
@@ -4404,18 +4414,18 @@
       <c r="D86" s="43">
         <v>20.548991199570501</v>
       </c>
-      <c r="E86" s="87"/>
+      <c r="E86" s="84"/>
       <c r="F86" s="44">
         <v>-24.697972040738954</v>
       </c>
-      <c r="G86" s="87"/>
+      <c r="G86" s="84"/>
       <c r="H86" s="43">
         <v>63.539104594429006</v>
       </c>
-      <c r="I86" s="87"/>
-      <c r="J86" s="46"/>
-    </row>
-    <row r="87" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I86" s="84"/>
+      <c r="J86" s="45"/>
+    </row>
+    <row r="87" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="42" t="s">
         <v>58</v>
       </c>
@@ -4425,18 +4435,18 @@
       <c r="D87" s="43">
         <v>85.66</v>
       </c>
-      <c r="E87" s="87"/>
+      <c r="E87" s="84"/>
       <c r="F87" s="44">
         <v>-28.912863070539423</v>
       </c>
-      <c r="G87" s="87"/>
+      <c r="G87" s="84"/>
       <c r="H87" s="43">
         <v>0.40493441754783621</v>
       </c>
-      <c r="I87" s="87"/>
-      <c r="J87" s="46"/>
-    </row>
-    <row r="88" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I87" s="84"/>
+      <c r="J87" s="45"/>
+    </row>
+    <row r="88" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="42" t="s">
         <v>59</v>
       </c>
@@ -4446,18 +4456,18 @@
       <c r="D88" s="43">
         <v>600.83699999999999</v>
       </c>
-      <c r="E88" s="87"/>
+      <c r="E88" s="84"/>
       <c r="F88" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G88" s="87"/>
+      <c r="G88" s="84"/>
       <c r="H88" s="43">
         <v>9.1243194273681922</v>
       </c>
-      <c r="I88" s="87"/>
-      <c r="J88" s="46"/>
-    </row>
-    <row r="89" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I88" s="84"/>
+      <c r="J88" s="45"/>
+    </row>
+    <row r="89" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="36"/>
       <c r="B89" s="37" t="s">
         <v>60</v>
@@ -4479,7 +4489,7 @@
       <c r="I89" s="41"/>
       <c r="J89" s="40"/>
     </row>
-    <row r="90" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="36"/>
       <c r="B90" s="37" t="s">
         <v>61</v>
@@ -4501,7 +4511,7 @@
       <c r="I90" s="41"/>
       <c r="J90" s="40"/>
     </row>
-    <row r="91" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="36"/>
       <c r="B91" s="37" t="s">
         <v>62</v>
@@ -4523,7 +4533,7 @@
       <c r="I91" s="41"/>
       <c r="J91" s="40"/>
     </row>
-    <row r="92" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="36"/>
       <c r="B92" s="37" t="s">
         <v>63</v>
@@ -4545,7 +4555,7 @@
       <c r="I92" s="41"/>
       <c r="J92" s="40"/>
     </row>
-    <row r="93" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="36"/>
       <c r="B93" s="37" t="s">
         <v>64</v>
@@ -4567,7 +4577,7 @@
       <c r="I93" s="41"/>
       <c r="J93" s="40"/>
     </row>
-    <row r="94" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="42" t="s">
         <v>65</v>
       </c>
@@ -4577,18 +4587,18 @@
       <c r="D94" s="43">
         <v>116</v>
       </c>
-      <c r="E94" s="87"/>
+      <c r="E94" s="84"/>
       <c r="F94" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G94" s="87"/>
+      <c r="G94" s="84"/>
       <c r="H94" s="43">
         <v>20.975664973785847</v>
       </c>
-      <c r="I94" s="87"/>
-      <c r="J94" s="46"/>
-    </row>
-    <row r="95" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I94" s="84"/>
+      <c r="J94" s="45"/>
+    </row>
+    <row r="95" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="42" t="s">
         <v>143</v>
       </c>
@@ -4598,18 +4608,18 @@
       <c r="D95" s="43">
         <v>500.26406679182099</v>
       </c>
-      <c r="E95" s="87"/>
+      <c r="E95" s="84"/>
       <c r="F95" s="44">
         <v>-25.889766032780543</v>
       </c>
-      <c r="G95" s="87"/>
+      <c r="G95" s="84"/>
       <c r="H95" s="43">
         <v>29.739643020881424</v>
       </c>
-      <c r="I95" s="87"/>
-      <c r="J95" s="46"/>
-    </row>
-    <row r="96" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I95" s="84"/>
+      <c r="J95" s="45"/>
+    </row>
+    <row r="96" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="42" t="s">
         <v>66</v>
       </c>
@@ -4619,18 +4629,18 @@
       <c r="D96" s="43">
         <v>49.975569</v>
       </c>
-      <c r="E96" s="87"/>
+      <c r="E96" s="84"/>
       <c r="F96" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G96" s="87"/>
+      <c r="G96" s="84"/>
       <c r="H96" s="43">
         <v>1.8782096301617153</v>
       </c>
-      <c r="I96" s="87"/>
-      <c r="J96" s="46"/>
-    </row>
-    <row r="97" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I96" s="84"/>
+      <c r="J96" s="45"/>
+    </row>
+    <row r="97" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="42" t="s">
         <v>67</v>
       </c>
@@ -4640,18 +4650,18 @@
       <c r="D97" s="43">
         <v>2.4485900000000001E-7</v>
       </c>
-      <c r="E97" s="87"/>
+      <c r="E97" s="84"/>
       <c r="F97" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G97" s="87"/>
+      <c r="G97" s="84"/>
       <c r="H97" s="43">
         <v>3.1935075775360616E-6</v>
       </c>
-      <c r="I97" s="87"/>
-      <c r="J97" s="46"/>
-    </row>
-    <row r="98" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I97" s="84"/>
+      <c r="J97" s="45"/>
+    </row>
+    <row r="98" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="42" t="s">
         <v>167</v>
       </c>
@@ -4661,18 +4671,18 @@
       <c r="D98" s="43">
         <v>113</v>
       </c>
-      <c r="E98" s="87"/>
+      <c r="E98" s="84"/>
       <c r="F98" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G98" s="87"/>
+      <c r="G98" s="84"/>
       <c r="H98" s="43">
         <v>66.789172588541462</v>
       </c>
-      <c r="I98" s="87"/>
-      <c r="J98" s="46"/>
-    </row>
-    <row r="99" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I98" s="84"/>
+      <c r="J98" s="45"/>
+    </row>
+    <row r="99" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="36"/>
       <c r="B99" s="37" t="s">
         <v>68</v>
@@ -4694,7 +4704,7 @@
       <c r="I99" s="41"/>
       <c r="J99" s="40"/>
     </row>
-    <row r="100" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="36"/>
       <c r="B100" s="37" t="s">
         <v>168</v>
@@ -4716,7 +4726,7 @@
       <c r="I100" s="41"/>
       <c r="J100" s="40"/>
     </row>
-    <row r="101" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="36"/>
       <c r="B101" s="37" t="s">
         <v>69</v>
@@ -4738,7 +4748,7 @@
       <c r="I101" s="41"/>
       <c r="J101" s="40"/>
     </row>
-    <row r="102" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="36"/>
       <c r="B102" s="37" t="s">
         <v>70</v>
@@ -4760,10 +4770,10 @@
       <c r="I102" s="41"/>
       <c r="J102" s="40"/>
     </row>
-    <row r="103" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="36"/>
       <c r="B103" s="37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C103" s="37">
         <v>1998</v>
@@ -4782,7 +4792,7 @@
       <c r="I103" s="41"/>
       <c r="J103" s="40"/>
     </row>
-    <row r="104" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="36"/>
       <c r="B104" s="37" t="s">
         <v>169</v>
@@ -4804,7 +4814,7 @@
       <c r="I104" s="41"/>
       <c r="J104" s="40"/>
     </row>
-    <row r="105" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="42" t="s">
         <v>71</v>
       </c>
@@ -4814,18 +4824,18 @@
       <c r="D105" s="43">
         <v>59.531692308580801</v>
       </c>
-      <c r="E105" s="87"/>
+      <c r="E105" s="84"/>
       <c r="F105" s="44">
         <v>-63.393109902319964</v>
       </c>
-      <c r="G105" s="87"/>
+      <c r="G105" s="84"/>
       <c r="H105" s="43">
         <v>19.735379164627037</v>
       </c>
-      <c r="I105" s="87"/>
-      <c r="J105" s="46"/>
-    </row>
-    <row r="106" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I105" s="84"/>
+      <c r="J105" s="45"/>
+    </row>
+    <row r="106" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="42" t="s">
         <v>72</v>
       </c>
@@ -4835,18 +4845,18 @@
       <c r="D106" s="43">
         <v>0.44</v>
       </c>
-      <c r="E106" s="87"/>
+      <c r="E106" s="84"/>
       <c r="F106" s="44">
         <v>175.00000000000003</v>
       </c>
-      <c r="G106" s="87"/>
+      <c r="G106" s="84"/>
       <c r="H106" s="43">
         <v>0.96101972929821533</v>
       </c>
-      <c r="I106" s="87"/>
-      <c r="J106" s="46"/>
-    </row>
-    <row r="107" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I106" s="84"/>
+      <c r="J106" s="45"/>
+    </row>
+    <row r="107" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="42" t="s">
         <v>73</v>
       </c>
@@ -4856,18 +4866,18 @@
       <c r="D107" s="43">
         <v>27.64</v>
       </c>
-      <c r="E107" s="87"/>
+      <c r="E107" s="84"/>
       <c r="F107" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G107" s="87"/>
+      <c r="G107" s="84"/>
       <c r="H107" s="43">
         <v>1.7554990021791943</v>
       </c>
-      <c r="I107" s="87"/>
-      <c r="J107" s="46"/>
-    </row>
-    <row r="108" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I107" s="84"/>
+      <c r="J107" s="45"/>
+    </row>
+    <row r="108" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="42" t="s">
         <v>74</v>
       </c>
@@ -4877,18 +4887,18 @@
       <c r="D108" s="43">
         <v>26.31</v>
       </c>
-      <c r="E108" s="87"/>
+      <c r="E108" s="84"/>
       <c r="F108" s="44">
         <v>-8.9934278796264309</v>
       </c>
-      <c r="G108" s="87"/>
+      <c r="G108" s="84"/>
       <c r="H108" s="43">
         <v>2.7052282159724244</v>
       </c>
-      <c r="I108" s="87"/>
-      <c r="J108" s="46"/>
-    </row>
-    <row r="109" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I108" s="84"/>
+      <c r="J108" s="45"/>
+    </row>
+    <row r="109" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="42" t="s">
         <v>75</v>
       </c>
@@ -4898,18 +4908,18 @@
       <c r="D109" s="43">
         <v>42.54</v>
       </c>
-      <c r="E109" s="87"/>
+      <c r="E109" s="84"/>
       <c r="F109" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G109" s="87"/>
+      <c r="G109" s="84"/>
       <c r="H109" s="43">
         <v>3.8508450224071384</v>
       </c>
-      <c r="I109" s="87"/>
-      <c r="J109" s="46"/>
-    </row>
-    <row r="110" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I109" s="84"/>
+      <c r="J109" s="45"/>
+    </row>
+    <row r="110" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="36"/>
       <c r="B110" s="37" t="s">
         <v>76</v>
@@ -4931,7 +4941,7 @@
       <c r="I110" s="41"/>
       <c r="J110" s="40"/>
     </row>
-    <row r="111" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="36"/>
       <c r="B111" s="37" t="s">
         <v>77</v>
@@ -4953,7 +4963,7 @@
       <c r="I111" s="41"/>
       <c r="J111" s="40"/>
     </row>
-    <row r="112" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="36"/>
       <c r="B112" s="37" t="s">
         <v>170</v>
@@ -4975,7 +4985,7 @@
       <c r="I112" s="41"/>
       <c r="J112" s="40"/>
     </row>
-    <row r="113" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="36"/>
       <c r="B113" s="37" t="s">
         <v>78</v>
@@ -4997,7 +5007,7 @@
       <c r="I113" s="41"/>
       <c r="J113" s="40"/>
     </row>
-    <row r="114" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="36"/>
       <c r="B114" s="37" t="s">
         <v>171</v>
@@ -5019,7 +5029,7 @@
       <c r="I114" s="41"/>
       <c r="J114" s="40"/>
     </row>
-    <row r="115" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="42" t="s">
         <v>79</v>
       </c>
@@ -5029,18 +5039,18 @@
       <c r="D115" s="43">
         <v>0.334060734477933</v>
       </c>
-      <c r="E115" s="87"/>
+      <c r="E115" s="84"/>
       <c r="F115" s="44">
         <v>-26.163329932244757</v>
       </c>
-      <c r="G115" s="87"/>
+      <c r="G115" s="84"/>
       <c r="H115" s="43">
         <v>8.931149996736524</v>
       </c>
-      <c r="I115" s="87"/>
-      <c r="J115" s="46"/>
-    </row>
-    <row r="116" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I115" s="84"/>
+      <c r="J115" s="45"/>
+    </row>
+    <row r="116" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B116" s="42" t="s">
         <v>80</v>
       </c>
@@ -5050,18 +5060,18 @@
       <c r="D116" s="43">
         <v>2.98</v>
       </c>
-      <c r="E116" s="87"/>
+      <c r="E116" s="84"/>
       <c r="F116" s="44">
         <v>29.565217391304355</v>
       </c>
-      <c r="G116" s="87"/>
+      <c r="G116" s="84"/>
       <c r="H116" s="43">
         <v>1.2650769149783407</v>
       </c>
-      <c r="I116" s="87"/>
-      <c r="J116" s="46"/>
-    </row>
-    <row r="117" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I116" s="84"/>
+      <c r="J116" s="45"/>
+    </row>
+    <row r="117" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="42" t="s">
         <v>172</v>
       </c>
@@ -5071,18 +5081,18 @@
       <c r="D117" s="43">
         <v>10.94</v>
       </c>
-      <c r="E117" s="87"/>
+      <c r="E117" s="84"/>
       <c r="F117" s="44">
         <v>5.802707930367502</v>
       </c>
-      <c r="G117" s="87"/>
+      <c r="G117" s="84"/>
       <c r="H117" s="43">
         <v>17.808250396371932</v>
       </c>
-      <c r="I117" s="87"/>
-      <c r="J117" s="46"/>
-    </row>
-    <row r="118" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I117" s="84"/>
+      <c r="J117" s="45"/>
+    </row>
+    <row r="118" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="42" t="s">
         <v>81</v>
       </c>
@@ -5092,18 +5102,18 @@
       <c r="D118" s="43">
         <v>190.91</v>
       </c>
-      <c r="E118" s="87"/>
+      <c r="E118" s="84"/>
       <c r="F118" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G118" s="87"/>
+      <c r="G118" s="84"/>
       <c r="H118" s="43">
         <v>6.4637271013131246</v>
       </c>
-      <c r="I118" s="87"/>
-      <c r="J118" s="46"/>
-    </row>
-    <row r="119" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I118" s="84"/>
+      <c r="J118" s="45"/>
+    </row>
+    <row r="119" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="42" t="s">
         <v>82</v>
       </c>
@@ -5113,18 +5123,18 @@
       <c r="D119" s="43">
         <v>93.81</v>
       </c>
-      <c r="E119" s="87"/>
+      <c r="E119" s="84"/>
       <c r="F119" s="44">
         <v>22.08485163977095</v>
       </c>
-      <c r="G119" s="87"/>
+      <c r="G119" s="84"/>
       <c r="H119" s="43">
         <v>6.1062034170915771</v>
       </c>
-      <c r="I119" s="87"/>
-      <c r="J119" s="46"/>
-    </row>
-    <row r="120" spans="1:10" s="47" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I119" s="84"/>
+      <c r="J119" s="45"/>
+    </row>
+    <row r="120" spans="1:10" s="46" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="36"/>
       <c r="B120" s="37" t="s">
         <v>173</v>
@@ -5146,7 +5156,7 @@
       <c r="I120" s="41"/>
       <c r="J120" s="40"/>
     </row>
-    <row r="121" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="36"/>
       <c r="B121" s="37" t="s">
         <v>83</v>
@@ -5168,7 +5178,7 @@
       <c r="I121" s="41"/>
       <c r="J121" s="40"/>
     </row>
-    <row r="122" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="36"/>
       <c r="B122" s="37" t="s">
         <v>84</v>
@@ -5190,7 +5200,7 @@
       <c r="I122" s="41"/>
       <c r="J122" s="40"/>
     </row>
-    <row r="123" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="36"/>
       <c r="B123" s="37" t="s">
         <v>85</v>
@@ -5212,7 +5222,7 @@
       <c r="I123" s="41"/>
       <c r="J123" s="40"/>
     </row>
-    <row r="124" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="36"/>
       <c r="B124" s="37" t="s">
         <v>86</v>
@@ -5234,7 +5244,7 @@
       <c r="I124" s="41"/>
       <c r="J124" s="40"/>
     </row>
-    <row r="125" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="42" t="s">
         <v>144</v>
       </c>
@@ -5244,18 +5254,18 @@
       <c r="D125" s="43">
         <v>24</v>
       </c>
-      <c r="E125" s="87"/>
+      <c r="E125" s="84"/>
       <c r="F125" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G125" s="87"/>
+      <c r="G125" s="84"/>
       <c r="H125" s="43">
         <v>2.1381754930699506</v>
       </c>
-      <c r="I125" s="87"/>
-      <c r="J125" s="46"/>
-    </row>
-    <row r="126" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I125" s="84"/>
+      <c r="J125" s="45"/>
+    </row>
+    <row r="126" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="42" t="s">
         <v>87</v>
       </c>
@@ -5265,18 +5275,18 @@
       <c r="D126" s="43">
         <v>1008</v>
       </c>
-      <c r="E126" s="87"/>
+      <c r="E126" s="84"/>
       <c r="F126" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G126" s="87"/>
+      <c r="G126" s="84"/>
       <c r="H126" s="43">
         <v>8.2033437691856417</v>
       </c>
-      <c r="I126" s="87"/>
-      <c r="J126" s="46"/>
-    </row>
-    <row r="127" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I126" s="84"/>
+      <c r="J126" s="45"/>
+    </row>
+    <row r="127" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="42" t="s">
         <v>88</v>
       </c>
@@ -5286,22 +5296,22 @@
       <c r="D127" s="43">
         <v>26.3005</v>
       </c>
-      <c r="E127" s="87">
+      <c r="E127" s="84">
         <v>3</v>
       </c>
       <c r="F127" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G127" s="87"/>
+      <c r="G127" s="84"/>
       <c r="H127" s="43">
         <v>11938.49296413981</v>
       </c>
-      <c r="I127" s="87">
+      <c r="I127" s="84">
         <v>3</v>
       </c>
-      <c r="J127" s="46"/>
-    </row>
-    <row r="128" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J127" s="45"/>
+    </row>
+    <row r="128" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="42" t="s">
         <v>89</v>
       </c>
@@ -5311,18 +5321,18 @@
       <c r="D128" s="43">
         <v>166.22842089950001</v>
       </c>
-      <c r="E128" s="87"/>
+      <c r="E128" s="84"/>
       <c r="F128" s="44">
         <v>-13.274263856272931</v>
       </c>
-      <c r="G128" s="87"/>
+      <c r="G128" s="84"/>
       <c r="H128" s="43">
         <v>33.124006454589711</v>
       </c>
-      <c r="I128" s="87"/>
-      <c r="J128" s="46"/>
-    </row>
-    <row r="129" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I128" s="84"/>
+      <c r="J128" s="45"/>
+    </row>
+    <row r="129" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B129" s="42" t="s">
         <v>174</v>
       </c>
@@ -5332,18 +5342,18 @@
       <c r="D129" s="43">
         <v>0.218</v>
       </c>
-      <c r="E129" s="87"/>
+      <c r="E129" s="84"/>
       <c r="F129" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G129" s="87"/>
+      <c r="G129" s="84"/>
       <c r="H129" s="43">
         <v>0.10189110831819377</v>
       </c>
-      <c r="I129" s="87"/>
-      <c r="J129" s="46"/>
-    </row>
-    <row r="130" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I129" s="84"/>
+      <c r="J129" s="45"/>
+    </row>
+    <row r="130" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="36"/>
       <c r="B130" s="37" t="s">
         <v>90</v>
@@ -5365,7 +5375,7 @@
       <c r="I130" s="41"/>
       <c r="J130" s="40"/>
     </row>
-    <row r="131" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="36"/>
       <c r="B131" s="37" t="s">
         <v>191</v>
@@ -5387,7 +5397,7 @@
       <c r="I131" s="41"/>
       <c r="J131" s="40"/>
     </row>
-    <row r="132" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="36"/>
       <c r="B132" s="37" t="s">
         <v>91</v>
@@ -5409,7 +5419,7 @@
       <c r="I132" s="41"/>
       <c r="J132" s="40"/>
     </row>
-    <row r="133" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="36"/>
       <c r="B133" s="37" t="s">
         <v>92</v>
@@ -5431,7 +5441,7 @@
       <c r="I133" s="41"/>
       <c r="J133" s="40"/>
     </row>
-    <row r="134" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="36"/>
       <c r="B134" s="37" t="s">
         <v>93</v>
@@ -5453,7 +5463,7 @@
       <c r="I134" s="41"/>
       <c r="J134" s="40"/>
     </row>
-    <row r="135" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B135" s="42" t="s">
         <v>94</v>
       </c>
@@ -5463,18 +5473,18 @@
       <c r="D135" s="43">
         <v>817.3</v>
       </c>
-      <c r="E135" s="87"/>
+      <c r="E135" s="84"/>
       <c r="F135" s="44">
         <v>-36.1484375</v>
       </c>
-      <c r="G135" s="87"/>
+      <c r="G135" s="84"/>
       <c r="H135" s="43">
         <v>21.168372974455036</v>
       </c>
-      <c r="I135" s="87"/>
-      <c r="J135" s="46"/>
-    </row>
-    <row r="136" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I135" s="84"/>
+      <c r="J135" s="45"/>
+    </row>
+    <row r="136" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="42" t="s">
         <v>95</v>
       </c>
@@ -5484,18 +5494,18 @@
       <c r="D136" s="43">
         <v>172.135836186483</v>
       </c>
-      <c r="E136" s="87"/>
+      <c r="E136" s="84"/>
       <c r="F136" s="44">
         <v>-30.435374750944799</v>
       </c>
-      <c r="G136" s="87"/>
+      <c r="G136" s="84"/>
       <c r="H136" s="43">
         <v>16.370477818244215</v>
       </c>
-      <c r="I136" s="87"/>
-      <c r="J136" s="46"/>
-    </row>
-    <row r="137" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I136" s="84"/>
+      <c r="J136" s="45"/>
+    </row>
+    <row r="137" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="42" t="s">
         <v>175</v>
       </c>
@@ -5505,18 +5515,18 @@
       <c r="D137" s="43">
         <v>175.69</v>
       </c>
-      <c r="E137" s="87"/>
+      <c r="E137" s="84"/>
       <c r="F137" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G137" s="87"/>
+      <c r="G137" s="84"/>
       <c r="H137" s="43">
         <v>149.02180320707748</v>
       </c>
-      <c r="I137" s="87"/>
-      <c r="J137" s="46"/>
-    </row>
-    <row r="138" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I137" s="84"/>
+      <c r="J137" s="45"/>
+    </row>
+    <row r="138" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="42" t="s">
         <v>96</v>
       </c>
@@ -5526,18 +5536,18 @@
       <c r="D138" s="43">
         <v>37.063499999999998</v>
       </c>
-      <c r="E138" s="87"/>
+      <c r="E138" s="84"/>
       <c r="F138" s="44">
         <v>-72.989606425913536</v>
       </c>
-      <c r="G138" s="87"/>
+      <c r="G138" s="84"/>
       <c r="H138" s="43">
         <v>9.0742206541195038</v>
       </c>
-      <c r="I138" s="87"/>
-      <c r="J138" s="46"/>
-    </row>
-    <row r="139" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I138" s="84"/>
+      <c r="J138" s="45"/>
+    </row>
+    <row r="139" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="42" t="s">
         <v>97</v>
       </c>
@@ -5547,18 +5557,18 @@
       <c r="D139" s="43">
         <v>207.03701218098399</v>
       </c>
-      <c r="E139" s="87"/>
+      <c r="E139" s="84"/>
       <c r="F139" s="44">
         <v>-54.686770937502985</v>
       </c>
-      <c r="G139" s="87"/>
+      <c r="G139" s="84"/>
       <c r="H139" s="43">
         <v>10.380420640778816</v>
       </c>
-      <c r="I139" s="87"/>
-      <c r="J139" s="46"/>
-    </row>
-    <row r="140" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I139" s="84"/>
+      <c r="J139" s="45"/>
+    </row>
+    <row r="140" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="36"/>
       <c r="B140" s="37" t="s">
         <v>98</v>
@@ -5580,7 +5590,7 @@
       <c r="I140" s="41"/>
       <c r="J140" s="40"/>
     </row>
-    <row r="141" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="36"/>
       <c r="B141" s="37" t="s">
         <v>99</v>
@@ -5602,7 +5612,7 @@
       <c r="I141" s="41"/>
       <c r="J141" s="40"/>
     </row>
-    <row r="142" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="36"/>
       <c r="B142" s="37" t="s">
         <v>100</v>
@@ -5624,7 +5634,7 @@
       <c r="I142" s="41"/>
       <c r="J142" s="40"/>
     </row>
-    <row r="143" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="36"/>
       <c r="B143" s="37" t="s">
         <v>176</v>
@@ -5648,7 +5658,7 @@
       </c>
       <c r="J143" s="40"/>
     </row>
-    <row r="144" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="36"/>
       <c r="B144" s="37" t="s">
         <v>101</v>
@@ -5670,7 +5680,7 @@
       <c r="I144" s="41"/>
       <c r="J144" s="40"/>
     </row>
-    <row r="145" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B145" s="42" t="s">
         <v>145</v>
       </c>
@@ -5680,18 +5690,18 @@
       <c r="D145" s="43">
         <v>1.542</v>
       </c>
-      <c r="E145" s="87"/>
+      <c r="E145" s="84"/>
       <c r="F145" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G145" s="87"/>
+      <c r="G145" s="84"/>
       <c r="H145" s="43">
         <v>51.616790520184779</v>
       </c>
-      <c r="I145" s="87"/>
-      <c r="J145" s="46"/>
-    </row>
-    <row r="146" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I145" s="84"/>
+      <c r="J145" s="45"/>
+    </row>
+    <row r="146" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="42" t="s">
         <v>102</v>
       </c>
@@ -5701,18 +5711,18 @@
       <c r="D146" s="43">
         <v>0.77</v>
       </c>
-      <c r="E146" s="87"/>
+      <c r="E146" s="84"/>
       <c r="F146" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G146" s="87"/>
+      <c r="G146" s="84"/>
       <c r="H146" s="43">
         <v>5.0278818904835907</v>
       </c>
-      <c r="I146" s="87"/>
-      <c r="J146" s="46"/>
-    </row>
-    <row r="147" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I146" s="84"/>
+      <c r="J146" s="45"/>
+    </row>
+    <row r="147" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="42" t="s">
         <v>103</v>
       </c>
@@ -5722,18 +5732,18 @@
       <c r="D147" s="43">
         <v>8.4600000000000009</v>
       </c>
-      <c r="E147" s="87"/>
+      <c r="E147" s="84"/>
       <c r="F147" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G147" s="87"/>
+      <c r="G147" s="84"/>
       <c r="H147" s="43">
         <v>0.8579618760685227</v>
       </c>
-      <c r="I147" s="87"/>
-      <c r="J147" s="46"/>
-    </row>
-    <row r="148" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I147" s="84"/>
+      <c r="J147" s="45"/>
+    </row>
+    <row r="148" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B148" s="42" t="s">
         <v>177</v>
       </c>
@@ -5743,18 +5753,18 @@
       <c r="D148" s="43">
         <v>164</v>
       </c>
-      <c r="E148" s="87"/>
+      <c r="E148" s="84"/>
       <c r="F148" s="44">
         <v>-20.87996912389039</v>
       </c>
-      <c r="G148" s="87"/>
+      <c r="G148" s="84"/>
       <c r="H148" s="43">
         <v>16.960286455101574</v>
       </c>
-      <c r="I148" s="87"/>
-      <c r="J148" s="46"/>
-    </row>
-    <row r="149" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I148" s="84"/>
+      <c r="J148" s="45"/>
+    </row>
+    <row r="149" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B149" s="42" t="s">
         <v>104</v>
       </c>
@@ -5764,18 +5774,18 @@
       <c r="D149" s="43">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E149" s="87"/>
+      <c r="E149" s="84"/>
       <c r="F149" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G149" s="87"/>
+      <c r="G149" s="84"/>
       <c r="H149" s="43">
         <v>14.170589250067771</v>
       </c>
-      <c r="I149" s="87"/>
-      <c r="J149" s="46"/>
-    </row>
-    <row r="150" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I149" s="84"/>
+      <c r="J149" s="45"/>
+    </row>
+    <row r="150" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="36"/>
       <c r="B150" s="37" t="s">
         <v>105</v>
@@ -5797,7 +5807,7 @@
       <c r="I150" s="41"/>
       <c r="J150" s="40"/>
     </row>
-    <row r="151" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="36"/>
       <c r="B151" s="37" t="s">
         <v>106</v>
@@ -5819,7 +5829,7 @@
       <c r="I151" s="41"/>
       <c r="J151" s="40"/>
     </row>
-    <row r="152" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="36"/>
       <c r="B152" s="37" t="s">
         <v>107</v>
@@ -5841,7 +5851,7 @@
       <c r="I152" s="41"/>
       <c r="J152" s="40"/>
     </row>
-    <row r="153" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="36"/>
       <c r="B153" s="37" t="s">
         <v>108</v>
@@ -5863,7 +5873,7 @@
       <c r="I153" s="41"/>
       <c r="J153" s="40"/>
     </row>
-    <row r="154" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="36"/>
       <c r="B154" s="37" t="s">
         <v>109</v>
@@ -5885,7 +5895,7 @@
       <c r="I154" s="41"/>
       <c r="J154" s="40"/>
     </row>
-    <row r="155" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B155" s="42" t="s">
         <v>110</v>
       </c>
@@ -5895,18 +5905,18 @@
       <c r="D155" s="43">
         <v>10</v>
       </c>
-      <c r="E155" s="87"/>
+      <c r="E155" s="84"/>
       <c r="F155" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G155" s="87"/>
+      <c r="G155" s="84"/>
       <c r="H155" s="43">
         <v>20.506889289456794</v>
       </c>
-      <c r="I155" s="87"/>
-      <c r="J155" s="46"/>
-    </row>
-    <row r="156" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I155" s="84"/>
+      <c r="J155" s="45"/>
+    </row>
+    <row r="156" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="42" t="s">
         <v>111</v>
       </c>
@@ -5916,18 +5926,18 @@
       <c r="D156" s="43">
         <v>19.930599999999998</v>
       </c>
-      <c r="E156" s="87"/>
+      <c r="E156" s="84"/>
       <c r="F156" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G156" s="87"/>
+      <c r="G156" s="84"/>
       <c r="H156" s="43">
         <v>21.107937425798777</v>
       </c>
-      <c r="I156" s="87"/>
-      <c r="J156" s="46"/>
-    </row>
-    <row r="157" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I156" s="84"/>
+      <c r="J156" s="45"/>
+    </row>
+    <row r="157" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="42" t="s">
         <v>112</v>
       </c>
@@ -5937,18 +5947,18 @@
       <c r="D157" s="43">
         <v>131.81196688424299</v>
       </c>
-      <c r="E157" s="87"/>
+      <c r="E157" s="84"/>
       <c r="F157" s="44">
         <v>-51.187333619969777</v>
       </c>
-      <c r="G157" s="87"/>
+      <c r="G157" s="84"/>
       <c r="H157" s="43">
         <v>13.811763062823355</v>
       </c>
-      <c r="I157" s="87"/>
-      <c r="J157" s="46"/>
-    </row>
-    <row r="158" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I157" s="84"/>
+      <c r="J157" s="45"/>
+    </row>
+    <row r="158" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B158" s="42" t="s">
         <v>113</v>
       </c>
@@ -5958,18 +5968,18 @@
       <c r="D158" s="43">
         <v>73.711184660278406</v>
       </c>
-      <c r="E158" s="87"/>
+      <c r="E158" s="84"/>
       <c r="F158" s="44">
         <v>-49.135286695113543</v>
       </c>
-      <c r="G158" s="87"/>
+      <c r="G158" s="84"/>
       <c r="H158" s="43">
         <v>9.1879100788766994</v>
       </c>
-      <c r="I158" s="87"/>
-      <c r="J158" s="46"/>
-    </row>
-    <row r="159" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I158" s="84"/>
+      <c r="J158" s="45"/>
+    </row>
+    <row r="159" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B159" s="42" t="s">
         <v>114</v>
       </c>
@@ -5979,18 +5989,18 @@
       <c r="D159" s="43">
         <v>6</v>
       </c>
-      <c r="E159" s="87"/>
+      <c r="E159" s="84"/>
       <c r="F159" s="44">
         <v>-91.891891891891902</v>
       </c>
-      <c r="G159" s="87"/>
+      <c r="G159" s="84"/>
       <c r="H159" s="43">
         <v>0.79137965964343593</v>
       </c>
-      <c r="I159" s="87"/>
-      <c r="J159" s="46"/>
-    </row>
-    <row r="160" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I159" s="84"/>
+      <c r="J159" s="45"/>
+    </row>
+    <row r="160" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="36"/>
       <c r="B160" s="37" t="s">
         <v>115</v>
@@ -6012,7 +6022,7 @@
       <c r="I160" s="41"/>
       <c r="J160" s="40"/>
     </row>
-    <row r="161" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="36"/>
       <c r="B161" s="37" t="s">
         <v>178</v>
@@ -6034,7 +6044,7 @@
       <c r="I161" s="41"/>
       <c r="J161" s="40"/>
     </row>
-    <row r="162" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="36"/>
       <c r="B162" s="37" t="s">
         <v>179</v>
@@ -6056,7 +6066,7 @@
       <c r="I162" s="41"/>
       <c r="J162" s="40"/>
     </row>
-    <row r="163" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="36"/>
       <c r="B163" s="37" t="s">
         <v>116</v>
@@ -6078,7 +6088,7 @@
       <c r="I163" s="41"/>
       <c r="J163" s="40"/>
     </row>
-    <row r="164" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="36"/>
       <c r="B164" s="37" t="s">
         <v>117</v>
@@ -6100,7 +6110,7 @@
       <c r="I164" s="41"/>
       <c r="J164" s="40"/>
     </row>
-    <row r="165" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="42" t="s">
         <v>118</v>
       </c>
@@ -6110,18 +6120,18 @@
       <c r="D165" s="43">
         <v>36.857999999999997</v>
       </c>
-      <c r="E165" s="87"/>
+      <c r="E165" s="84"/>
       <c r="F165" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G165" s="87"/>
+      <c r="G165" s="84"/>
       <c r="H165" s="43">
         <v>30.164399167201349</v>
       </c>
-      <c r="I165" s="87"/>
-      <c r="J165" s="46"/>
-    </row>
-    <row r="166" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I165" s="84"/>
+      <c r="J165" s="45"/>
+    </row>
+    <row r="166" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="42" t="s">
         <v>119</v>
       </c>
@@ -6131,18 +6141,18 @@
       <c r="D166" s="43">
         <v>94.873800000000003</v>
       </c>
-      <c r="E166" s="87"/>
+      <c r="E166" s="84"/>
       <c r="F166" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G166" s="87"/>
+      <c r="G166" s="84"/>
       <c r="H166" s="43">
         <v>9.7816189224834407</v>
       </c>
-      <c r="I166" s="87"/>
-      <c r="J166" s="46"/>
-    </row>
-    <row r="167" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I166" s="84"/>
+      <c r="J166" s="45"/>
+    </row>
+    <row r="167" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B167" s="42" t="s">
         <v>120</v>
       </c>
@@ -6152,18 +6162,18 @@
       <c r="D167" s="43">
         <v>1283.73692305449</v>
       </c>
-      <c r="E167" s="87"/>
+      <c r="E167" s="84"/>
       <c r="F167" s="44">
         <v>99.427127355598003</v>
       </c>
-      <c r="G167" s="87"/>
+      <c r="G167" s="84"/>
       <c r="H167" s="43">
         <v>17.150980184387173</v>
       </c>
-      <c r="I167" s="87"/>
-      <c r="J167" s="46"/>
-    </row>
-    <row r="168" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I167" s="84"/>
+      <c r="J167" s="45"/>
+    </row>
+    <row r="168" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="42" t="s">
         <v>121</v>
       </c>
@@ -6173,18 +6183,18 @@
       <c r="D168" s="43">
         <v>90.239000000000004</v>
       </c>
-      <c r="E168" s="87"/>
+      <c r="E168" s="84"/>
       <c r="F168" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G168" s="87"/>
+      <c r="G168" s="84"/>
       <c r="H168" s="43">
         <v>19.21255745308158</v>
       </c>
-      <c r="I168" s="87"/>
-      <c r="J168" s="46"/>
-    </row>
-    <row r="169" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I168" s="84"/>
+      <c r="J168" s="45"/>
+    </row>
+    <row r="169" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B169" s="42" t="s">
         <v>122</v>
       </c>
@@ -6194,18 +6204,18 @@
       <c r="D169" s="43">
         <v>6.9699999999999995E-8</v>
       </c>
-      <c r="E169" s="87"/>
+      <c r="E169" s="84"/>
       <c r="F169" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G169" s="87"/>
+      <c r="G169" s="84"/>
       <c r="H169" s="43">
         <v>7.5859817152808005E-6</v>
       </c>
-      <c r="I169" s="87"/>
-      <c r="J169" s="46"/>
-    </row>
-    <row r="170" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I169" s="84"/>
+      <c r="J169" s="45"/>
+    </row>
+    <row r="170" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="36"/>
       <c r="B170" s="37" t="s">
         <v>123</v>
@@ -6227,7 +6237,7 @@
       <c r="I170" s="41"/>
       <c r="J170" s="40"/>
     </row>
-    <row r="171" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="36"/>
       <c r="B171" s="37" t="s">
         <v>124</v>
@@ -6249,7 +6259,7 @@
       <c r="I171" s="41"/>
       <c r="J171" s="40"/>
     </row>
-    <row r="172" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="36"/>
       <c r="B172" s="37" t="s">
         <v>125</v>
@@ -6271,7 +6281,7 @@
       <c r="I172" s="41"/>
       <c r="J172" s="40"/>
     </row>
-    <row r="173" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="36"/>
       <c r="B173" s="37" t="s">
         <v>180</v>
@@ -6293,7 +6303,7 @@
       <c r="I173" s="41"/>
       <c r="J173" s="40"/>
     </row>
-    <row r="174" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="36"/>
       <c r="B174" s="37" t="s">
         <v>181</v>
@@ -6319,7 +6329,7 @@
       <c r="I174" s="41"/>
       <c r="J174" s="40"/>
     </row>
-    <row r="175" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="42" t="s">
         <v>182</v>
       </c>
@@ -6329,18 +6339,18 @@
       <c r="D175" s="43">
         <v>11882.0219961603</v>
       </c>
-      <c r="E175" s="87"/>
+      <c r="E175" s="84"/>
       <c r="F175" s="44">
         <v>-45.451048903972591</v>
       </c>
-      <c r="G175" s="87"/>
+      <c r="G175" s="84"/>
       <c r="H175" s="43">
         <v>37.744733766178094</v>
       </c>
-      <c r="I175" s="87"/>
-      <c r="J175" s="46"/>
-    </row>
-    <row r="176" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I175" s="84"/>
+      <c r="J175" s="45"/>
+    </row>
+    <row r="176" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="42" t="s">
         <v>126</v>
       </c>
@@ -6350,18 +6360,18 @@
       <c r="D176" s="43">
         <v>38.757330000000003</v>
       </c>
-      <c r="E176" s="87"/>
+      <c r="E176" s="84"/>
       <c r="F176" s="44">
         <v>29.229868960688222</v>
       </c>
-      <c r="G176" s="87"/>
+      <c r="G176" s="84"/>
       <c r="H176" s="43">
         <v>11.659509833651015</v>
       </c>
-      <c r="I176" s="87"/>
-      <c r="J176" s="46"/>
-    </row>
-    <row r="177" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I176" s="84"/>
+      <c r="J176" s="45"/>
+    </row>
+    <row r="177" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B177" s="42" t="s">
         <v>127</v>
       </c>
@@ -6371,18 +6381,18 @@
       <c r="D177" s="43">
         <v>257.524</v>
       </c>
-      <c r="E177" s="87"/>
+      <c r="E177" s="84"/>
       <c r="F177" s="44">
         <v>-37.482794197972936</v>
       </c>
-      <c r="G177" s="87"/>
+      <c r="G177" s="84"/>
       <c r="H177" s="43">
         <v>9.9344813540219263</v>
       </c>
-      <c r="I177" s="87"/>
-      <c r="J177" s="46"/>
-    </row>
-    <row r="178" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I177" s="84"/>
+      <c r="J177" s="45"/>
+    </row>
+    <row r="178" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B178" s="42" t="s">
         <v>128</v>
       </c>
@@ -6392,18 +6402,18 @@
       <c r="D178" s="43">
         <v>8.3230898999999997E-2</v>
       </c>
-      <c r="E178" s="87"/>
+      <c r="E178" s="84"/>
       <c r="F178" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G178" s="87"/>
+      <c r="G178" s="84"/>
       <c r="H178" s="43">
         <v>0.50685954484833351</v>
       </c>
-      <c r="I178" s="87"/>
-      <c r="J178" s="46"/>
-    </row>
-    <row r="179" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I178" s="84"/>
+      <c r="J178" s="45"/>
+    </row>
+    <row r="179" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B179" s="42" t="s">
         <v>146</v>
       </c>
@@ -6413,18 +6423,18 @@
       <c r="D179" s="43">
         <v>395.79</v>
       </c>
-      <c r="E179" s="87"/>
+      <c r="E179" s="84"/>
       <c r="F179" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G179" s="87"/>
+      <c r="G179" s="84"/>
       <c r="H179" s="43">
         <v>16.475217553917847</v>
       </c>
-      <c r="I179" s="87"/>
-      <c r="J179" s="46"/>
-    </row>
-    <row r="180" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I179" s="84"/>
+      <c r="J179" s="45"/>
+    </row>
+    <row r="180" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="36"/>
       <c r="B180" s="37" t="s">
         <v>129</v>
@@ -6446,7 +6456,7 @@
       <c r="I180" s="41"/>
       <c r="J180" s="40"/>
     </row>
-    <row r="181" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="36"/>
       <c r="B181" s="37" t="s">
         <v>130</v>
@@ -6468,7 +6478,7 @@
       <c r="I181" s="41"/>
       <c r="J181" s="40"/>
     </row>
-    <row r="182" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="36"/>
       <c r="B182" s="37" t="s">
         <v>131</v>
@@ -6494,7 +6504,7 @@
       </c>
       <c r="J182" s="40"/>
     </row>
-    <row r="183" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="36"/>
       <c r="B183" s="37" t="s">
         <v>132</v>
@@ -6516,421 +6526,411 @@
       <c r="I183" s="41"/>
       <c r="J183" s="40"/>
     </row>
-    <row r="184" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="48"/>
-      <c r="B184" s="48"/>
-      <c r="C184" s="48"/>
-      <c r="D184" s="49"/>
-      <c r="E184" s="48"/>
-      <c r="F184" s="50"/>
-      <c r="G184" s="48"/>
-      <c r="H184" s="49"/>
-      <c r="I184" s="48"/>
+    <row r="184" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="47"/>
+      <c r="B184" s="47"/>
+      <c r="C184" s="47"/>
+      <c r="D184" s="48"/>
+      <c r="E184" s="47"/>
+      <c r="F184" s="49"/>
+      <c r="G184" s="47"/>
+      <c r="H184" s="48"/>
+      <c r="I184" s="47"/>
       <c r="J184" s="35"/>
     </row>
-    <row r="185" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="45"/>
-      <c r="C185" s="45"/>
-      <c r="D185" s="51"/>
-      <c r="E185" s="45"/>
-      <c r="F185" s="52"/>
-      <c r="G185" s="45"/>
-      <c r="H185" s="51"/>
-      <c r="I185" s="45"/>
-    </row>
-    <row r="186" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="53" t="s">
+    <row r="185" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B185" s="42"/>
+      <c r="C185" s="42"/>
+      <c r="D185" s="43"/>
+      <c r="E185" s="42"/>
+      <c r="F185" s="44"/>
+      <c r="G185" s="42"/>
+      <c r="H185" s="43"/>
+      <c r="I185" s="42"/>
+    </row>
+    <row r="186" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="50" t="s">
         <v>133</v>
       </c>
       <c r="C186" s="16"/>
-      <c r="D186" s="54"/>
+      <c r="D186" s="51"/>
       <c r="E186" s="16"/>
       <c r="F186" s="8"/>
       <c r="G186" s="16"/>
-      <c r="H186" s="54"/>
-    </row>
-    <row r="187" spans="1:10" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="53"/>
+      <c r="H186" s="51"/>
+    </row>
+    <row r="187" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="50"/>
       <c r="C187" s="16"/>
-      <c r="D187" s="54"/>
+      <c r="D187" s="51"/>
       <c r="E187" s="16"/>
       <c r="F187" s="8"/>
       <c r="G187" s="16"/>
-      <c r="H187" s="54"/>
-    </row>
-    <row r="188" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="103" t="s">
+      <c r="H187" s="51"/>
+    </row>
+    <row r="188" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="102" t="s">
+        <v>192</v>
+      </c>
+      <c r="B188" s="102"/>
+      <c r="C188" s="102"/>
+      <c r="D188" s="102"/>
+      <c r="E188" s="102"/>
+      <c r="F188" s="102"/>
+      <c r="G188" s="102"/>
+      <c r="H188" s="102"/>
+      <c r="I188" s="102"/>
+      <c r="J188" s="52"/>
+    </row>
+    <row r="189" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="95" t="s">
         <v>193</v>
       </c>
-      <c r="B188" s="103"/>
-      <c r="C188" s="103"/>
-      <c r="D188" s="103"/>
-      <c r="E188" s="103"/>
-      <c r="F188" s="103"/>
-      <c r="G188" s="103"/>
-      <c r="H188" s="103"/>
-      <c r="I188" s="103"/>
-      <c r="J188" s="55"/>
-    </row>
-    <row r="189" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="109" t="s">
+      <c r="B189" s="95"/>
+      <c r="C189" s="89"/>
+      <c r="D189" s="89"/>
+      <c r="E189" s="89"/>
+      <c r="F189" s="89"/>
+      <c r="G189" s="89"/>
+      <c r="H189" s="89"/>
+      <c r="I189" s="89"/>
+      <c r="J189" s="52"/>
+    </row>
+    <row r="190" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="102" t="s">
+        <v>197</v>
+      </c>
+      <c r="B190" s="102"/>
+      <c r="C190" s="102"/>
+      <c r="D190" s="102"/>
+      <c r="E190" s="102"/>
+      <c r="F190" s="102"/>
+      <c r="G190" s="102"/>
+      <c r="H190" s="102"/>
+      <c r="I190" s="102"/>
+      <c r="J190"/>
+    </row>
+    <row r="191" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="104" t="s">
         <v>194</v>
       </c>
-      <c r="B189" s="109"/>
-      <c r="C189" s="92"/>
-      <c r="D189" s="92"/>
-      <c r="E189" s="92"/>
-      <c r="F189" s="92"/>
-      <c r="G189" s="92"/>
-      <c r="H189" s="92"/>
-      <c r="I189" s="92"/>
-      <c r="J189" s="55"/>
-    </row>
-    <row r="190" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="103" t="s">
+      <c r="B191" s="104"/>
+      <c r="C191" s="104"/>
+      <c r="D191" s="104"/>
+      <c r="E191" s="104"/>
+      <c r="F191" s="104"/>
+      <c r="G191" s="104"/>
+      <c r="H191" s="104"/>
+      <c r="I191" s="104"/>
+      <c r="J191"/>
+    </row>
+    <row r="192" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="53"/>
+      <c r="B192" s="54"/>
+      <c r="C192" s="54"/>
+      <c r="D192" s="55"/>
+      <c r="E192" s="54"/>
+      <c r="F192" s="54"/>
+      <c r="G192" s="54"/>
+      <c r="H192" s="55"/>
+      <c r="I192" s="54"/>
+    </row>
+    <row r="193" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="105" t="s">
+        <v>134</v>
+      </c>
+      <c r="B193" s="105"/>
+      <c r="C193" s="105"/>
+      <c r="D193" s="105"/>
+      <c r="E193" s="105"/>
+      <c r="F193" s="105"/>
+      <c r="G193" s="105"/>
+      <c r="H193" s="105"/>
+    </row>
+    <row r="194" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="56"/>
+      <c r="B194" s="56"/>
+      <c r="C194" s="56"/>
+      <c r="D194" s="56"/>
+      <c r="E194" s="56"/>
+      <c r="F194" s="56"/>
+      <c r="G194" s="56"/>
+      <c r="H194" s="56"/>
+    </row>
+    <row r="195" spans="1:9" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="85">
+        <v>1</v>
+      </c>
+      <c r="B195" s="103" t="s">
+        <v>185</v>
+      </c>
+      <c r="C195" s="103"/>
+      <c r="D195" s="103"/>
+      <c r="E195" s="103"/>
+      <c r="F195" s="103"/>
+      <c r="G195" s="103"/>
+      <c r="H195" s="103"/>
+      <c r="I195" s="103"/>
+    </row>
+    <row r="196" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="85">
+        <v>2</v>
+      </c>
+      <c r="B196" s="103" t="s">
+        <v>186</v>
+      </c>
+      <c r="C196" s="103"/>
+      <c r="D196" s="103"/>
+      <c r="E196" s="103"/>
+      <c r="F196" s="103"/>
+      <c r="G196" s="103"/>
+      <c r="H196" s="103"/>
+      <c r="I196" s="103"/>
+    </row>
+    <row r="197" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="85">
+        <v>3</v>
+      </c>
+      <c r="B197" s="103" t="s">
+        <v>187</v>
+      </c>
+      <c r="C197" s="103"/>
+      <c r="D197" s="103"/>
+      <c r="E197" s="103"/>
+      <c r="F197" s="103"/>
+      <c r="G197" s="103"/>
+      <c r="H197" s="103"/>
+      <c r="I197" s="103"/>
+    </row>
+    <row r="198" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="85">
+        <v>4</v>
+      </c>
+      <c r="B198" s="103" t="s">
+        <v>188</v>
+      </c>
+      <c r="C198" s="103"/>
+      <c r="D198" s="103"/>
+      <c r="E198" s="103"/>
+      <c r="F198" s="103"/>
+      <c r="G198" s="103"/>
+      <c r="H198" s="103"/>
+      <c r="I198" s="103"/>
+    </row>
+    <row r="199" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="85">
+        <v>5</v>
+      </c>
+      <c r="B199" s="103" t="s">
+        <v>201</v>
+      </c>
+      <c r="C199" s="103"/>
+      <c r="D199" s="103"/>
+      <c r="E199" s="103"/>
+      <c r="F199" s="103"/>
+      <c r="G199" s="103"/>
+      <c r="H199" s="103"/>
+      <c r="I199" s="103"/>
+    </row>
+    <row r="200" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="85">
+        <v>6</v>
+      </c>
+      <c r="B200" s="103" t="s">
+        <v>189</v>
+      </c>
+      <c r="C200" s="103"/>
+      <c r="D200" s="103"/>
+      <c r="E200" s="103"/>
+      <c r="F200" s="103"/>
+      <c r="G200" s="103"/>
+      <c r="H200" s="103"/>
+      <c r="I200" s="103"/>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B201" s="17"/>
+      <c r="C201" s="53"/>
+      <c r="D201" s="57"/>
+      <c r="E201" s="53"/>
+      <c r="F201" s="53"/>
+      <c r="G201" s="53"/>
+      <c r="H201" s="57"/>
+      <c r="I201" s="53"/>
+    </row>
+    <row r="202" spans="1:9" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="97" t="s">
+        <v>135</v>
+      </c>
+      <c r="B202" s="97"/>
+      <c r="C202" s="97"/>
+      <c r="D202" s="97"/>
+      <c r="E202" s="54"/>
+      <c r="F202" s="54"/>
+      <c r="G202" s="54"/>
+      <c r="H202" s="55"/>
+    </row>
+    <row r="203" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="58"/>
+      <c r="B203" s="54"/>
+      <c r="C203" s="54"/>
+      <c r="D203" s="55"/>
+      <c r="E203" s="54"/>
+      <c r="F203" s="54"/>
+      <c r="G203" s="54"/>
+      <c r="H203" s="55"/>
+    </row>
+    <row r="204" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="92" t="s">
+        <v>150</v>
+      </c>
+      <c r="B204" s="92"/>
+      <c r="C204" s="92"/>
+      <c r="D204" s="92"/>
+      <c r="E204" s="92"/>
+      <c r="F204" s="92"/>
+      <c r="G204" s="92"/>
+      <c r="H204" s="92"/>
+      <c r="I204" s="92"/>
+    </row>
+    <row r="205" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="B205" s="93"/>
+      <c r="C205" s="93"/>
+      <c r="D205" s="93"/>
+      <c r="E205" s="93"/>
+      <c r="F205" s="93"/>
+      <c r="G205" s="93"/>
+      <c r="H205" s="93"/>
+      <c r="I205" s="93"/>
+    </row>
+    <row r="206" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="96" t="s">
         <v>198</v>
       </c>
-      <c r="B190" s="103"/>
-      <c r="C190" s="103"/>
-      <c r="D190" s="103"/>
-      <c r="E190" s="103"/>
-      <c r="F190" s="103"/>
-      <c r="G190" s="103"/>
-      <c r="H190" s="103"/>
-      <c r="I190" s="103"/>
-      <c r="J190" s="93"/>
-    </row>
-    <row r="191" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="105" t="s">
-        <v>195</v>
-      </c>
-      <c r="B191" s="105"/>
-      <c r="C191" s="105"/>
-      <c r="D191" s="105"/>
-      <c r="E191" s="105"/>
-      <c r="F191" s="105"/>
-      <c r="G191" s="105"/>
-      <c r="H191" s="105"/>
-      <c r="I191" s="105"/>
-      <c r="J191" s="93"/>
-    </row>
-    <row r="192" spans="1:10" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="56"/>
-      <c r="B192" s="57"/>
-      <c r="C192" s="57"/>
-      <c r="D192" s="58"/>
-      <c r="E192" s="57"/>
-      <c r="F192" s="57"/>
-      <c r="G192" s="57"/>
-      <c r="H192" s="58"/>
-      <c r="I192" s="57"/>
-    </row>
-    <row r="193" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="106" t="s">
-        <v>134</v>
-      </c>
-      <c r="B193" s="106"/>
-      <c r="C193" s="106"/>
-      <c r="D193" s="106"/>
-      <c r="E193" s="106"/>
-      <c r="F193" s="106"/>
-      <c r="G193" s="106"/>
-      <c r="H193" s="106"/>
-    </row>
-    <row r="194" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="59"/>
-      <c r="B194" s="59"/>
-      <c r="C194" s="59"/>
-      <c r="D194" s="59"/>
-      <c r="E194" s="59"/>
-      <c r="F194" s="59"/>
-      <c r="G194" s="59"/>
-      <c r="H194" s="59"/>
-    </row>
-    <row r="195" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="88">
-        <v>1</v>
-      </c>
-      <c r="B195" s="104" t="s">
-        <v>185</v>
-      </c>
-      <c r="C195" s="104"/>
-      <c r="D195" s="104"/>
-      <c r="E195" s="104"/>
-      <c r="F195" s="104"/>
-      <c r="G195" s="104"/>
-      <c r="H195" s="104"/>
-      <c r="I195" s="104"/>
-    </row>
-    <row r="196" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="88">
-        <v>2</v>
-      </c>
-      <c r="B196" s="104" t="s">
-        <v>186</v>
-      </c>
-      <c r="C196" s="104"/>
-      <c r="D196" s="104"/>
-      <c r="E196" s="104"/>
-      <c r="F196" s="104"/>
-      <c r="G196" s="104"/>
-      <c r="H196" s="104"/>
-      <c r="I196" s="104"/>
-    </row>
-    <row r="197" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="88">
-        <v>3</v>
-      </c>
-      <c r="B197" s="104" t="s">
-        <v>187</v>
-      </c>
-      <c r="C197" s="104"/>
-      <c r="D197" s="104"/>
-      <c r="E197" s="104"/>
-      <c r="F197" s="104"/>
-      <c r="G197" s="104"/>
-      <c r="H197" s="104"/>
-      <c r="I197" s="104"/>
-    </row>
-    <row r="198" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="88">
-        <v>4</v>
-      </c>
-      <c r="B198" s="104" t="s">
-        <v>188</v>
-      </c>
-      <c r="C198" s="104"/>
-      <c r="D198" s="104"/>
-      <c r="E198" s="104"/>
-      <c r="F198" s="104"/>
-      <c r="G198" s="104"/>
-      <c r="H198" s="104"/>
-      <c r="I198" s="104"/>
-    </row>
-    <row r="199" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="88">
-        <v>5</v>
-      </c>
-      <c r="B199" s="104" t="s">
+      <c r="B206" s="96"/>
+      <c r="C206" s="96"/>
+      <c r="D206" s="96"/>
+      <c r="E206" s="96"/>
+      <c r="F206" s="96"/>
+      <c r="G206" s="96"/>
+      <c r="H206" s="96"/>
+      <c r="I206" s="96"/>
+    </row>
+    <row r="207" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="93" t="s">
         <v>202</v>
       </c>
-      <c r="C199" s="104"/>
-      <c r="D199" s="104"/>
-      <c r="E199" s="104"/>
-      <c r="F199" s="104"/>
-      <c r="G199" s="104"/>
-      <c r="H199" s="104"/>
-      <c r="I199" s="104"/>
-    </row>
-    <row r="200" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="88">
-        <v>6</v>
-      </c>
-      <c r="B200" s="104" t="s">
-        <v>189</v>
-      </c>
-      <c r="C200" s="104"/>
-      <c r="D200" s="104"/>
-      <c r="E200" s="104"/>
-      <c r="F200" s="104"/>
-      <c r="G200" s="104"/>
-      <c r="H200" s="104"/>
-      <c r="I200" s="104"/>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B201" s="17"/>
-      <c r="C201" s="56"/>
-      <c r="D201" s="60"/>
-      <c r="E201" s="56"/>
-      <c r="F201" s="56"/>
-      <c r="G201" s="56"/>
-      <c r="H201" s="60"/>
-      <c r="I201" s="56"/>
-    </row>
-    <row r="202" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="101" t="s">
-        <v>135</v>
-      </c>
-      <c r="B202" s="101"/>
-      <c r="C202" s="101"/>
-      <c r="D202" s="101"/>
-      <c r="E202" s="57"/>
-      <c r="F202" s="57"/>
-      <c r="G202" s="57"/>
-      <c r="H202" s="58"/>
-    </row>
-    <row r="203" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="61"/>
-      <c r="B203" s="57"/>
-      <c r="C203" s="57"/>
-      <c r="D203" s="58"/>
-      <c r="E203" s="57"/>
-      <c r="F203" s="57"/>
-      <c r="G203" s="57"/>
-      <c r="H203" s="58"/>
-    </row>
-    <row r="204" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="102" t="s">
-        <v>150</v>
-      </c>
-      <c r="B204" s="102"/>
-      <c r="C204" s="102"/>
-      <c r="D204" s="102"/>
-      <c r="E204" s="102"/>
-      <c r="F204" s="102"/>
-      <c r="G204" s="102"/>
-      <c r="H204" s="102"/>
-      <c r="I204" s="102"/>
-    </row>
-    <row r="205" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="107" t="s">
+      <c r="B207" s="93"/>
+      <c r="C207" s="93"/>
+      <c r="D207" s="93"/>
+      <c r="E207" s="93"/>
+      <c r="F207" s="93"/>
+      <c r="G207" s="93"/>
+      <c r="H207" s="93"/>
+      <c r="I207" s="93"/>
+    </row>
+    <row r="208" spans="1:9" s="91" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="96" t="s">
         <v>200</v>
       </c>
-      <c r="B205" s="107"/>
-      <c r="C205" s="107"/>
-      <c r="D205" s="107"/>
-      <c r="E205" s="107"/>
-      <c r="F205" s="107"/>
-      <c r="G205" s="107"/>
-      <c r="H205" s="107"/>
-      <c r="I205" s="107"/>
-    </row>
-    <row r="206" spans="1:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="110" t="s">
-        <v>199</v>
-      </c>
-      <c r="B206" s="110"/>
-      <c r="C206" s="110"/>
-      <c r="D206" s="110"/>
-      <c r="E206" s="110"/>
-      <c r="F206" s="110"/>
-      <c r="G206" s="110"/>
-      <c r="H206" s="110"/>
-      <c r="I206" s="110"/>
-    </row>
-    <row r="207" spans="1:9" s="94" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="107" t="s">
-        <v>203</v>
-      </c>
-      <c r="B207" s="107"/>
-      <c r="C207" s="107"/>
-      <c r="D207" s="107"/>
-      <c r="E207" s="107"/>
-      <c r="F207" s="107"/>
-      <c r="G207" s="107"/>
-      <c r="H207" s="107"/>
-      <c r="I207" s="107"/>
-    </row>
-    <row r="208" spans="1:9" s="96" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="110" t="s">
-        <v>201</v>
-      </c>
-      <c r="B208" s="110"/>
-      <c r="C208" s="110"/>
-      <c r="D208" s="110"/>
-      <c r="E208" s="110"/>
-      <c r="F208" s="110"/>
-      <c r="G208" s="110"/>
-      <c r="H208" s="110"/>
-      <c r="I208" s="110"/>
-    </row>
-    <row r="209" spans="1:9" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="107" t="s">
+      <c r="B208" s="96"/>
+      <c r="C208" s="96"/>
+      <c r="D208" s="96"/>
+      <c r="E208" s="96"/>
+      <c r="F208" s="96"/>
+      <c r="G208" s="96"/>
+      <c r="H208" s="96"/>
+      <c r="I208" s="96"/>
+    </row>
+    <row r="209" spans="1:9" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="93" t="s">
         <v>151</v>
       </c>
-      <c r="B209" s="107"/>
-      <c r="C209" s="107"/>
-      <c r="D209" s="107"/>
-      <c r="E209" s="107"/>
-      <c r="F209" s="107"/>
-      <c r="G209" s="107"/>
-      <c r="H209" s="107"/>
-      <c r="I209" s="107"/>
-    </row>
-    <row r="210" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="108" t="s">
+      <c r="B209" s="93"/>
+      <c r="C209" s="93"/>
+      <c r="D209" s="93"/>
+      <c r="E209" s="93"/>
+      <c r="F209" s="93"/>
+      <c r="G209" s="93"/>
+      <c r="H209" s="93"/>
+      <c r="I209" s="93"/>
+    </row>
+    <row r="210" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="94" t="s">
         <v>154</v>
       </c>
-      <c r="B210" s="107"/>
-      <c r="C210" s="107"/>
-      <c r="D210" s="107"/>
-      <c r="E210" s="107"/>
-      <c r="F210" s="107"/>
-      <c r="G210" s="107"/>
-      <c r="H210" s="107"/>
-      <c r="I210" s="107"/>
-    </row>
-    <row r="211" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="107" t="s">
+      <c r="B210" s="93"/>
+      <c r="C210" s="93"/>
+      <c r="D210" s="93"/>
+      <c r="E210" s="93"/>
+      <c r="F210" s="93"/>
+      <c r="G210" s="93"/>
+      <c r="H210" s="93"/>
+      <c r="I210" s="93"/>
+    </row>
+    <row r="211" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="93" t="s">
         <v>190</v>
       </c>
-      <c r="B211" s="107"/>
-      <c r="C211" s="107"/>
-      <c r="D211" s="107"/>
-      <c r="E211" s="107"/>
-      <c r="F211" s="107"/>
-      <c r="G211" s="107"/>
-      <c r="H211" s="107"/>
-      <c r="I211" s="107"/>
-    </row>
-    <row r="212" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="62"/>
-      <c r="B212" s="56"/>
-      <c r="C212" s="56"/>
-      <c r="D212" s="60"/>
-      <c r="E212" s="56"/>
-      <c r="F212" s="56"/>
-      <c r="G212" s="56"/>
-      <c r="H212" s="60"/>
-    </row>
-    <row r="213" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="101" t="s">
+      <c r="B211" s="93"/>
+      <c r="C211" s="93"/>
+      <c r="D211" s="93"/>
+      <c r="E211" s="93"/>
+      <c r="F211" s="93"/>
+      <c r="G211" s="93"/>
+      <c r="H211" s="93"/>
+      <c r="I211" s="93"/>
+    </row>
+    <row r="212" spans="1:9" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="59"/>
+      <c r="B212" s="53"/>
+      <c r="C212" s="53"/>
+      <c r="D212" s="57"/>
+      <c r="E212" s="53"/>
+      <c r="F212" s="53"/>
+      <c r="G212" s="53"/>
+      <c r="H212" s="57"/>
+    </row>
+    <row r="213" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="97" t="s">
         <v>136</v>
       </c>
-      <c r="B213" s="101"/>
-      <c r="C213" s="101"/>
-      <c r="D213" s="101"/>
-      <c r="E213" s="56"/>
-      <c r="F213" s="56"/>
-      <c r="G213" s="56"/>
-      <c r="H213" s="60"/>
-    </row>
-    <row r="214" spans="1:9" ht="4.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="91"/>
-      <c r="B214" s="91"/>
-      <c r="C214" s="91"/>
-      <c r="D214" s="91"/>
-      <c r="E214" s="56"/>
-      <c r="F214" s="56"/>
-      <c r="G214" s="56"/>
-      <c r="H214" s="60"/>
-    </row>
-    <row r="215" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="102" t="s">
+      <c r="B213" s="97"/>
+      <c r="C213" s="97"/>
+      <c r="D213" s="97"/>
+      <c r="E213" s="53"/>
+      <c r="F213" s="53"/>
+      <c r="G213" s="53"/>
+      <c r="H213" s="57"/>
+    </row>
+    <row r="214" spans="1:9" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="88"/>
+      <c r="B214" s="88"/>
+      <c r="C214" s="88"/>
+      <c r="D214" s="88"/>
+      <c r="E214" s="53"/>
+      <c r="F214" s="53"/>
+      <c r="G214" s="53"/>
+      <c r="H214" s="57"/>
+    </row>
+    <row r="215" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="92" t="s">
         <v>152</v>
       </c>
-      <c r="B215" s="102"/>
-      <c r="C215" s="102"/>
-      <c r="D215" s="102"/>
-      <c r="E215" s="102"/>
-      <c r="F215" s="102"/>
-      <c r="G215" s="102"/>
-      <c r="H215" s="102"/>
-      <c r="I215" s="102"/>
+      <c r="B215" s="92"/>
+      <c r="C215" s="92"/>
+      <c r="D215" s="92"/>
+      <c r="E215" s="92"/>
+      <c r="F215" s="92"/>
+      <c r="G215" s="92"/>
+      <c r="H215" s="92"/>
+      <c r="I215" s="92"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="A215:I215"/>
-    <mergeCell ref="A209:I209"/>
-    <mergeCell ref="A210:I210"/>
-    <mergeCell ref="A211:I211"/>
-    <mergeCell ref="A189:B189"/>
-    <mergeCell ref="A206:I206"/>
-    <mergeCell ref="A205:I205"/>
-    <mergeCell ref="A208:I208"/>
-    <mergeCell ref="A207:I207"/>
-    <mergeCell ref="A213:D213"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="A202:D202"/>
@@ -6945,17 +6945,27 @@
     <mergeCell ref="B198:I198"/>
     <mergeCell ref="B195:I195"/>
     <mergeCell ref="A190:I190"/>
+    <mergeCell ref="A215:I215"/>
+    <mergeCell ref="A209:I209"/>
+    <mergeCell ref="A210:I210"/>
+    <mergeCell ref="A211:I211"/>
+    <mergeCell ref="A189:B189"/>
+    <mergeCell ref="A206:I206"/>
+    <mergeCell ref="A205:I205"/>
+    <mergeCell ref="A208:I208"/>
+    <mergeCell ref="A207:I207"/>
+    <mergeCell ref="A213:D213"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:I7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:I7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$B$19:$B$183</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A189:B189" r:id="rId1" display="Available at: http://unfccc.int"/>
-    <hyperlink ref="A206:I206" r:id="rId2" display="See:  http://www.ipcc-nggip.iges.or.jp/public/gl/invs1.html ."/>
-    <hyperlink ref="A208:I208" r:id="rId3" display="See:  http://www.ipcc-nggip.iges.or.jp/public/2006gl/index.htm ."/>
+    <hyperlink ref="A189:B189" r:id="rId1" display="Available at: http://unfccc.int" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A206:I206" r:id="rId2" display="See:  http://www.ipcc-nggip.iges.or.jp/public/gl/invs1.html ." xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A208:I208" r:id="rId3" display="See:  http://www.ipcc-nggip.iges.or.jp/public/2006gl/index.htm ." xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.4" right="0.56000000000000005" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup scale="94" orientation="portrait" r:id="rId4"/>

</xml_diff>